<commit_message>
Update model, update function import file
</commit_message>
<xml_diff>
--- a/SEP-VanLangHotel/Upload/Demo.xlsx
+++ b/SEP-VanLangHotel/Upload/Demo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dangt\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB05841-29CC-4973-A11D-E33C53862E8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2053B517-0FFA-4F0B-B744-7CB3A3C01A7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{E93DE5FD-DC7B-498D-86AD-F192523F8D5C}"/>
   </bookViews>
@@ -36,17 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="102">
   <si>
     <t>STT</t>
   </si>
   <si>
-    <t>SL Người lớn</t>
-  </si>
-  <si>
-    <t>SL Trẻ em</t>
-  </si>
-  <si>
     <t>Số giường</t>
   </si>
   <si>
@@ -80,18 +74,6 @@
     <t>Diệp Thế Tài</t>
   </si>
   <si>
-    <t>0367909247</t>
-  </si>
-  <si>
-    <t>0367909246</t>
-  </si>
-  <si>
-    <t>0367909245</t>
-  </si>
-  <si>
-    <t>0367909244</t>
-  </si>
-  <si>
     <t>Bình Phước</t>
   </si>
   <si>
@@ -101,36 +83,6 @@
     <t>THÔNG TIN NGƯỜI ĐẶT PHÒNG</t>
   </si>
   <si>
-    <t>0367909243</t>
-  </si>
-  <si>
-    <t>0367909242</t>
-  </si>
-  <si>
-    <t>0367909241</t>
-  </si>
-  <si>
-    <t>0367909240</t>
-  </si>
-  <si>
-    <t>0367909239</t>
-  </si>
-  <si>
-    <t>0367909238</t>
-  </si>
-  <si>
-    <t>0367909237</t>
-  </si>
-  <si>
-    <t>0367909236</t>
-  </si>
-  <si>
-    <t>0367909235</t>
-  </si>
-  <si>
-    <t>0367909234</t>
-  </si>
-  <si>
     <t>Phòng hút thuốc</t>
   </si>
   <si>
@@ -249,37 +201,61 @@
   </si>
   <si>
     <t>Loại phòng</t>
-  </si>
-  <si>
-    <t>Ngày ở (YYYY-MM-DD)
-VD: 2022-05-30</t>
-  </si>
-  <si>
-    <t>Ngày đi (YYYY-MM-DD)
-VD: 2022-05-30</t>
   </si>
   <si>
     <t>Nam (1)
 Nữ (0)</t>
   </si>
   <si>
-    <t>Ngày sinh (YYYY-MM-DD)
+    <t>THÔNG TIN PHÒNG</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>F3</t>
+  </si>
+  <si>
+    <t>F4</t>
+  </si>
+  <si>
+    <t>Nếu số người lớn &lt;= 2 và trẻ em &lt;= 2</t>
+  </si>
+  <si>
+    <t>Nếu số người lớn = 3 người lớn và trẻ em &lt;= 3</t>
+  </si>
+  <si>
+    <t>Nếu số người lớn = 4 người lớn và trẻ em &lt;= 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nếu số người lớn &lt;= 2 và trẻ em từ &lt;= 4 </t>
+  </si>
+  <si>
+    <t>Ngày sinh (Năm-Tháng-Ngày)
 VD: 2000-02-20</t>
   </si>
   <si>
-    <t>THÔNG TIN PHÒNG</t>
-  </si>
-  <si>
-    <t>TIỆN ÍCH PHÒNG</t>
-  </si>
-  <si>
-    <t>F2</t>
-  </si>
-  <si>
-    <t>F3</t>
-  </si>
-  <si>
-    <t>F4</t>
+    <t>070200001923</t>
+  </si>
+  <si>
+    <t>0367909249</t>
+  </si>
+  <si>
+    <t>TIỆN ÍCH PHÒNG (CÓ: 1, KHÔNG: 0)</t>
+  </si>
+  <si>
+    <t>Số Trẻ em &lt; 14t</t>
+  </si>
+  <si>
+    <t>Số Người lớn</t>
+  </si>
+  <si>
+    <t>Ngày ở (Năm-Tháng-Ngày)
+VD: 2000-02-20</t>
+  </si>
+  <si>
+    <t>Ngày đi (Năm-Tháng-Ngày)
+VD: 2000-02-20</t>
   </si>
   <si>
     <r>
@@ -400,30 +376,7 @@
         <charset val="163"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Năm-Tháng-Ngày (YYYY-MM-DD)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
+      <t xml:space="preserve">Năm-Tháng-Ngày (VD: 2022-01-30)
 4. </t>
     </r>
     <r>
@@ -506,18 +459,140 @@
       </rPr>
       <t>.</t>
     </r>
-  </si>
-  <si>
-    <t>Nếu số người lớn &lt;= 2 và trẻ em &lt;= 2</t>
-  </si>
-  <si>
-    <t>Nếu số người lớn = 3 người lớn và trẻ em &lt;= 3</t>
-  </si>
-  <si>
-    <t>Nếu số người lớn = 4 người lớn và trẻ em &lt;= 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nếu số người lớn &lt;= 2 và trẻ em từ &lt;= 4 </t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+5. Ngày ở </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">và </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ngày đi</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> của tất cả các phòng phải đều giống nhau.</t>
+    </r>
+  </si>
+  <si>
+    <t>070200001922</t>
+  </si>
+  <si>
+    <t>070200001912</t>
+  </si>
+  <si>
+    <t>070200001913</t>
+  </si>
+  <si>
+    <t>070200001914</t>
+  </si>
+  <si>
+    <t>070200001915</t>
+  </si>
+  <si>
+    <t>070200001916</t>
+  </si>
+  <si>
+    <t>070200001917</t>
+  </si>
+  <si>
+    <t>070200001918</t>
+  </si>
+  <si>
+    <t>070200001919</t>
+  </si>
+  <si>
+    <t>070200001920</t>
+  </si>
+  <si>
+    <t>070200001924</t>
+  </si>
+  <si>
+    <t>070200001921</t>
+  </si>
+  <si>
+    <t>070200001925</t>
+  </si>
+  <si>
+    <t>070200001926</t>
+  </si>
+  <si>
+    <t>070200001927</t>
+  </si>
+  <si>
+    <t>0367909250</t>
+  </si>
+  <si>
+    <t>0367909251</t>
+  </si>
+  <si>
+    <t>0367909252</t>
+  </si>
+  <si>
+    <t>0367909253</t>
+  </si>
+  <si>
+    <t>0367909254</t>
+  </si>
+  <si>
+    <t>0367909255</t>
+  </si>
+  <si>
+    <t>0367909256</t>
+  </si>
+  <si>
+    <t>0367909257</t>
+  </si>
+  <si>
+    <t>0367909258</t>
+  </si>
+  <si>
+    <t>0367909259</t>
+  </si>
+  <si>
+    <t>0367909260</t>
+  </si>
+  <si>
+    <t>0367909261</t>
+  </si>
+  <si>
+    <t>0367909262</t>
+  </si>
+  <si>
+    <t>0367909263</t>
   </si>
 </sst>
 </file>
@@ -527,12 +602,20 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -616,7 +699,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -631,19 +714,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -665,8 +736,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -750,39 +827,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -791,61 +868,87 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1166,7 +1269,7 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1176,51 +1279,51 @@
     <col min="3" max="5" width="10.3984375" customWidth="1"/>
     <col min="6" max="6" width="11.09765625" customWidth="1"/>
     <col min="7" max="7" width="38.59765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="76.796875" customWidth="1"/>
+    <col min="8" max="8" width="78.3984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="B1" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="F1" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="G1" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="H1" s="19" t="s">
-        <v>69</v>
+      <c r="A1" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="25" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
     </row>
     <row r="3" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="C3" s="1">
         <v>2</v>
@@ -1235,18 +1338,18 @@
         <v>250000</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="H3" s="20" t="s">
-        <v>80</v>
+        <v>60</v>
+      </c>
+      <c r="H3" s="26" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="C4" s="1">
         <v>2</v>
@@ -1260,17 +1363,17 @@
       <c r="F4" s="2">
         <v>400000</v>
       </c>
-      <c r="G4" s="31" t="s">
-        <v>84</v>
-      </c>
-      <c r="H4" s="21"/>
+      <c r="G4" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H4" s="27"/>
     </row>
     <row r="5" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="C5" s="1">
         <v>3</v>
@@ -1285,16 +1388,16 @@
         <v>500000</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="H5" s="21"/>
+        <v>61</v>
+      </c>
+      <c r="H5" s="27"/>
     </row>
     <row r="6" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="C6" s="1">
         <v>4</v>
@@ -1309,26 +1412,26 @@
         <v>600000</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="H6" s="21"/>
+        <v>62</v>
+      </c>
+      <c r="H6" s="27"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="22"/>
+      <c r="A7" s="21"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="28"/>
     </row>
     <row r="8" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="C8" s="1">
         <v>2</v>
@@ -1343,16 +1446,16 @@
         <v>280000</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="C9" s="1">
         <v>2</v>
@@ -1366,17 +1469,17 @@
       <c r="F9" s="2">
         <v>430000</v>
       </c>
-      <c r="G9" s="31" t="s">
-        <v>84</v>
+      <c r="G9" s="9" t="s">
+        <v>63</v>
       </c>
       <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="C10" s="1">
         <v>3</v>
@@ -1391,16 +1494,16 @@
         <v>530000</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="C11" s="1">
         <v>4</v>
@@ -1415,26 +1518,26 @@
         <v>630000</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="24"/>
+      <c r="A12" s="21"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="30"/>
       <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C13" s="1">
         <v>2</v>
@@ -1449,16 +1552,16 @@
         <v>310000</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="H13" s="3"/>
     </row>
     <row r="14" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C14" s="1">
         <v>2</v>
@@ -1472,17 +1575,17 @@
       <c r="F14" s="2">
         <v>460000</v>
       </c>
-      <c r="G14" s="31" t="s">
-        <v>84</v>
+      <c r="G14" s="9" t="s">
+        <v>63</v>
       </c>
       <c r="H14" s="3"/>
     </row>
     <row r="15" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C15" s="1">
         <v>3</v>
@@ -1497,16 +1600,16 @@
         <v>560000</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C16" s="1">
         <v>4</v>
@@ -1521,26 +1624,26 @@
         <v>660000</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="H16" s="3"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="17"/>
+      <c r="A17" s="21"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="23"/>
       <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="C18" s="1">
         <v>2</v>
@@ -1555,16 +1658,16 @@
         <v>340000</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="H18" s="3"/>
     </row>
     <row r="19" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="C19" s="1">
         <v>2</v>
@@ -1578,17 +1681,17 @@
       <c r="F19" s="2">
         <v>490000</v>
       </c>
-      <c r="G19" s="31" t="s">
-        <v>84</v>
+      <c r="G19" s="9" t="s">
+        <v>63</v>
       </c>
       <c r="H19" s="3"/>
     </row>
     <row r="20" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="C20" s="1">
         <v>3</v>
@@ -1603,16 +1706,16 @@
         <v>590000</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="H20" s="3"/>
     </row>
     <row r="21" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="C21" s="1">
         <v>4</v>
@@ -1627,26 +1730,26 @@
         <v>690000</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="H21" s="3"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="15"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="17"/>
+      <c r="A22" s="21"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="23"/>
       <c r="H22" s="3"/>
     </row>
     <row r="23" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C23" s="1">
         <v>2</v>
@@ -1661,16 +1764,16 @@
         <v>370000</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="H23" s="3"/>
     </row>
     <row r="24" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C24" s="1">
         <v>2</v>
@@ -1684,17 +1787,17 @@
       <c r="F24" s="2">
         <v>520000</v>
       </c>
-      <c r="G24" s="31" t="s">
-        <v>84</v>
+      <c r="G24" s="9" t="s">
+        <v>63</v>
       </c>
       <c r="H24" s="3"/>
     </row>
     <row r="25" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C25" s="1">
         <v>3</v>
@@ -1709,16 +1812,16 @@
         <v>620000</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="H25" s="3"/>
     </row>
     <row r="26" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C26" s="1">
         <v>4</v>
@@ -1733,26 +1836,26 @@
         <v>720000</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="H26" s="3"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="15"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="17"/>
+      <c r="A27" s="21"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="23"/>
       <c r="H27" s="3"/>
     </row>
     <row r="28" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="C28" s="1">
         <v>2</v>
@@ -1767,16 +1870,16 @@
         <v>220000</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="H28" s="3"/>
     </row>
     <row r="29" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="C29" s="1">
         <v>2</v>
@@ -1790,17 +1893,17 @@
       <c r="F29" s="2">
         <v>370000</v>
       </c>
-      <c r="G29" s="31" t="s">
-        <v>84</v>
+      <c r="G29" s="9" t="s">
+        <v>63</v>
       </c>
       <c r="H29" s="3"/>
     </row>
     <row r="30" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="C30" s="1">
         <v>3</v>
@@ -1815,16 +1918,16 @@
         <v>470000</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="H30" s="3"/>
     </row>
     <row r="31" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="C31" s="1">
         <v>4</v>
@@ -1839,18 +1942,18 @@
         <v>570000</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="H31" s="3"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="18"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
+      <c r="A32" s="24"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="24"/>
       <c r="H32" s="3"/>
     </row>
   </sheetData>
@@ -1871,7 +1974,7 @@
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
   </mergeCells>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1879,23 +1982,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1EC22DE-93F5-4706-915E-304A5F11A983}">
-  <dimension ref="A1:Q17"/>
+  <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.296875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="12.796875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="20.8984375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="21.19921875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="12.59765625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.69921875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.09765625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.796875" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.59765625" style="20" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.8984375" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.8984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.796875" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.59765625" style="4" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15" style="4" customWidth="1"/>
     <col min="13" max="13" width="24.296875" style="4" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="22.19921875" style="4" bestFit="1" customWidth="1"/>
@@ -1906,875 +2011,928 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="36"/>
+    </row>
+    <row r="2" spans="1:17" ht="35.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="K2" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="L2" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="O2" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="P2" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q2" s="17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6">
+        <v>3</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0</v>
+      </c>
+      <c r="D3" s="6">
+        <v>2</v>
+      </c>
+      <c r="E3" s="18">
+        <v>44732</v>
+      </c>
+      <c r="F3" s="18">
+        <v>44739</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="7">
+        <v>36829</v>
+      </c>
+      <c r="K3" s="6">
+        <v>1</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="M3" s="6">
+        <v>1</v>
+      </c>
+      <c r="N3" s="6">
+        <v>1</v>
+      </c>
+      <c r="O3" s="6">
+        <v>1</v>
+      </c>
+      <c r="P3" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6">
+        <v>2</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1</v>
+      </c>
+      <c r="E4" s="18">
+        <v>44732</v>
+      </c>
+      <c r="F4" s="18">
+        <v>44739</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="J4" s="7">
+        <v>36615</v>
+      </c>
+      <c r="K4" s="6">
+        <v>1</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="M4" s="6">
+        <v>1</v>
+      </c>
+      <c r="N4" s="6">
+        <v>1</v>
+      </c>
+      <c r="O4" s="6">
+        <v>1</v>
+      </c>
+      <c r="P4" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6">
+        <v>3</v>
+      </c>
+      <c r="C5" s="6">
+        <v>1</v>
+      </c>
+      <c r="D5" s="6">
+        <v>2</v>
+      </c>
+      <c r="E5" s="18">
+        <v>44732</v>
+      </c>
+      <c r="F5" s="18">
+        <v>44739</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="26" t="s">
+      <c r="I5" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="J5" s="7">
+        <v>37178</v>
+      </c>
+      <c r="K5" s="6">
+        <v>0</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="M5" s="6">
+        <v>1</v>
+      </c>
+      <c r="N5" s="6">
+        <v>1</v>
+      </c>
+      <c r="O5" s="6">
+        <v>1</v>
+      </c>
+      <c r="P5" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6">
+        <v>2</v>
+      </c>
+      <c r="C6" s="6">
+        <v>1</v>
+      </c>
+      <c r="D6" s="6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="18">
+        <v>44732</v>
+      </c>
+      <c r="F6" s="18">
+        <v>44739</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
-    </row>
-    <row r="2" spans="1:17" ht="35.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="6" t="s">
+      <c r="I6" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="J6" s="7">
+        <v>36911</v>
+      </c>
+      <c r="K6" s="6">
+        <v>0</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="M6" s="6">
+        <v>0</v>
+      </c>
+      <c r="N6" s="6">
+        <v>1</v>
+      </c>
+      <c r="O6" s="6">
+        <v>0</v>
+      </c>
+      <c r="P6" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>5</v>
+      </c>
+      <c r="B7" s="6">
+        <v>2</v>
+      </c>
+      <c r="C7" s="6">
         <v>3</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="G2" s="8" t="s">
+      <c r="D7" s="6">
+        <v>2</v>
+      </c>
+      <c r="E7" s="18">
+        <v>44732</v>
+      </c>
+      <c r="F7" s="18">
+        <v>44739</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="J7" s="7">
+        <v>37230</v>
+      </c>
+      <c r="K7" s="6">
+        <v>1</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="M7" s="6">
+        <v>1</v>
+      </c>
+      <c r="N7" s="6">
+        <v>0</v>
+      </c>
+      <c r="O7" s="6">
+        <v>1</v>
+      </c>
+      <c r="P7" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6">
         <v>4</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="8" t="s">
+      <c r="C8" s="6">
+        <v>1</v>
+      </c>
+      <c r="D8" s="6">
+        <v>2</v>
+      </c>
+      <c r="E8" s="18">
+        <v>44732</v>
+      </c>
+      <c r="F8" s="18">
+        <v>44739</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="J8" s="7">
+        <v>37010</v>
+      </c>
+      <c r="K8" s="6">
+        <v>0</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="M8" s="6">
+        <v>0</v>
+      </c>
+      <c r="N8" s="6">
+        <v>1</v>
+      </c>
+      <c r="O8" s="6">
+        <v>0</v>
+      </c>
+      <c r="P8" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
         <v>7</v>
       </c>
-      <c r="J2" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="K2" s="9" t="s">
+      <c r="B9" s="6">
+        <v>2</v>
+      </c>
+      <c r="C9" s="6">
+        <v>2</v>
+      </c>
+      <c r="D9" s="6">
+        <v>2</v>
+      </c>
+      <c r="E9" s="18">
+        <v>44732</v>
+      </c>
+      <c r="F9" s="18">
+        <v>44739</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="J9" s="7">
+        <v>36790</v>
+      </c>
+      <c r="K9" s="6">
+        <v>1</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="M9" s="6">
+        <v>1</v>
+      </c>
+      <c r="N9" s="6">
+        <v>0</v>
+      </c>
+      <c r="O9" s="6">
+        <v>1</v>
+      </c>
+      <c r="P9" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>8</v>
+      </c>
+      <c r="B10" s="6">
+        <v>2</v>
+      </c>
+      <c r="C10" s="6">
+        <v>2</v>
+      </c>
+      <c r="D10" s="6">
+        <v>1</v>
+      </c>
+      <c r="E10" s="18">
+        <v>44732</v>
+      </c>
+      <c r="F10" s="18">
+        <v>44739</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="J10" s="7">
+        <v>36570</v>
+      </c>
+      <c r="K10" s="6">
+        <v>0</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="M10" s="6">
+        <v>0</v>
+      </c>
+      <c r="N10" s="6">
+        <v>1</v>
+      </c>
+      <c r="O10" s="6">
+        <v>1</v>
+      </c>
+      <c r="P10" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
+        <v>9</v>
+      </c>
+      <c r="B11" s="6">
+        <v>1</v>
+      </c>
+      <c r="C11" s="6">
+        <v>1</v>
+      </c>
+      <c r="D11" s="6">
+        <v>2</v>
+      </c>
+      <c r="E11" s="18">
+        <v>44732</v>
+      </c>
+      <c r="F11" s="18">
+        <v>44739</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="J11" s="7">
+        <v>36600</v>
+      </c>
+      <c r="K11" s="6">
+        <v>1</v>
+      </c>
+      <c r="L11" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="M11" s="6">
+        <v>0</v>
+      </c>
+      <c r="N11" s="6">
+        <v>1</v>
+      </c>
+      <c r="O11" s="6">
+        <v>0</v>
+      </c>
+      <c r="P11" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>10</v>
+      </c>
+      <c r="B12" s="6">
+        <v>3</v>
+      </c>
+      <c r="C12" s="6">
+        <v>3</v>
+      </c>
+      <c r="D12" s="6">
+        <v>2</v>
+      </c>
+      <c r="E12" s="18">
+        <v>44732</v>
+      </c>
+      <c r="F12" s="18">
+        <v>44739</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="J12" s="7">
+        <v>36630</v>
+      </c>
+      <c r="K12" s="6">
+        <v>0</v>
+      </c>
+      <c r="L12" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="M12" s="6">
+        <v>1</v>
+      </c>
+      <c r="N12" s="6">
+        <v>0</v>
+      </c>
+      <c r="O12" s="6">
+        <v>1</v>
+      </c>
+      <c r="P12" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>11</v>
+      </c>
+      <c r="B13" s="6">
+        <v>2</v>
+      </c>
+      <c r="C13" s="6">
+        <v>1</v>
+      </c>
+      <c r="D13" s="6">
+        <v>2</v>
+      </c>
+      <c r="E13" s="18">
+        <v>44732</v>
+      </c>
+      <c r="F13" s="18">
+        <v>44739</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="I13" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="J13" s="7">
+        <v>36660</v>
+      </c>
+      <c r="K13" s="6">
+        <v>1</v>
+      </c>
+      <c r="L13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="M13" s="6">
+        <v>0</v>
+      </c>
+      <c r="N13" s="6">
+        <v>0</v>
+      </c>
+      <c r="O13" s="6">
+        <v>1</v>
+      </c>
+      <c r="P13" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
+        <v>12</v>
+      </c>
+      <c r="B14" s="6">
+        <v>4</v>
+      </c>
+      <c r="C14" s="6">
+        <v>1</v>
+      </c>
+      <c r="D14" s="6">
+        <v>2</v>
+      </c>
+      <c r="E14" s="18">
+        <v>44732</v>
+      </c>
+      <c r="F14" s="18">
+        <v>44739</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="J14" s="7">
+        <v>36690</v>
+      </c>
+      <c r="K14" s="6">
+        <v>0</v>
+      </c>
+      <c r="L14" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="M14" s="6">
+        <v>0</v>
+      </c>
+      <c r="N14" s="6">
+        <v>1</v>
+      </c>
+      <c r="O14" s="6">
+        <v>0</v>
+      </c>
+      <c r="P14" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>13</v>
+      </c>
+      <c r="B15" s="6">
+        <v>2</v>
+      </c>
+      <c r="C15" s="6">
+        <v>1</v>
+      </c>
+      <c r="D15" s="6">
+        <v>2</v>
+      </c>
+      <c r="E15" s="18">
+        <v>44732</v>
+      </c>
+      <c r="F15" s="18">
+        <v>44739</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="I15" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="J15" s="7">
+        <v>36720</v>
+      </c>
+      <c r="K15" s="6">
+        <v>1</v>
+      </c>
+      <c r="L15" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="M15" s="6">
+        <v>1</v>
+      </c>
+      <c r="N15" s="6">
+        <v>1</v>
+      </c>
+      <c r="O15" s="6">
+        <v>0</v>
+      </c>
+      <c r="P15" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>14</v>
+      </c>
+      <c r="B16" s="6">
+        <v>1</v>
+      </c>
+      <c r="C16" s="6">
+        <v>2</v>
+      </c>
+      <c r="D16" s="6">
+        <v>2</v>
+      </c>
+      <c r="E16" s="18">
+        <v>44732</v>
+      </c>
+      <c r="F16" s="18">
+        <v>44739</v>
+      </c>
+      <c r="G16" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="N2" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="O2" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="P2" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q2" s="10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11">
-        <v>1</v>
-      </c>
-      <c r="B3" s="11">
-        <v>2</v>
-      </c>
-      <c r="C3" s="11">
-        <v>0</v>
-      </c>
-      <c r="D3" s="11">
-        <v>1</v>
-      </c>
-      <c r="E3" s="12">
+      <c r="H16" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="J16" s="7">
+        <v>36750</v>
+      </c>
+      <c r="K16" s="6">
+        <v>1</v>
+      </c>
+      <c r="L16" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="M16" s="6">
+        <v>0</v>
+      </c>
+      <c r="N16" s="6">
+        <v>1</v>
+      </c>
+      <c r="O16" s="6">
+        <v>0</v>
+      </c>
+      <c r="P16" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>15</v>
+      </c>
+      <c r="B17" s="6">
+        <v>3</v>
+      </c>
+      <c r="C17" s="6">
+        <v>2</v>
+      </c>
+      <c r="D17" s="6">
+        <v>2</v>
+      </c>
+      <c r="E17" s="18">
         <v>44732</v>
       </c>
-      <c r="F3" s="12">
-        <v>44765</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" s="11">
-        <v>70200000000</v>
-      </c>
-      <c r="I3" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="J3" s="12">
-        <v>36829</v>
-      </c>
-      <c r="K3" s="11">
-        <v>1</v>
-      </c>
-      <c r="L3" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="M3" s="11">
-        <v>1</v>
-      </c>
-      <c r="N3" s="11">
-        <v>1</v>
-      </c>
-      <c r="O3" s="11">
-        <v>1</v>
-      </c>
-      <c r="P3" s="11">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11">
-        <v>2</v>
-      </c>
-      <c r="B4" s="11">
-        <v>5</v>
-      </c>
-      <c r="C4" s="11">
-        <v>1</v>
-      </c>
-      <c r="D4" s="11">
-        <v>2</v>
-      </c>
-      <c r="E4" s="12">
-        <v>44735</v>
-      </c>
-      <c r="F4" s="12">
-        <v>44737</v>
-      </c>
-      <c r="G4" s="11" t="s">
+      <c r="F17" s="18">
+        <v>44739</v>
+      </c>
+      <c r="G17" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="11">
-        <v>70200000001</v>
-      </c>
-      <c r="I4" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" s="12">
-        <v>37178</v>
-      </c>
-      <c r="K4" s="11">
-        <v>0</v>
-      </c>
-      <c r="L4" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M4" s="11">
-        <v>1</v>
-      </c>
-      <c r="N4" s="11">
-        <v>1</v>
-      </c>
-      <c r="O4" s="11">
-        <v>1</v>
-      </c>
-      <c r="P4" s="11">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11">
-        <v>3</v>
-      </c>
-      <c r="B5" s="11">
-        <v>2</v>
-      </c>
-      <c r="C5" s="11">
-        <v>1</v>
-      </c>
-      <c r="D5" s="11">
-        <v>1</v>
-      </c>
-      <c r="E5" s="12">
-        <v>44734</v>
-      </c>
-      <c r="F5" s="12">
-        <v>44800</v>
-      </c>
-      <c r="G5" s="11" t="s">
+      <c r="H17" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="J17" s="7">
+        <v>36780</v>
+      </c>
+      <c r="K17" s="6">
+        <v>1</v>
+      </c>
+      <c r="L17" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="M17" s="6">
+        <v>1</v>
+      </c>
+      <c r="N17" s="6">
+        <v>0</v>
+      </c>
+      <c r="O17" s="6">
+        <v>0</v>
+      </c>
+      <c r="P17" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>16</v>
+      </c>
+      <c r="B18" s="6">
+        <v>2</v>
+      </c>
+      <c r="C18" s="6">
+        <v>1</v>
+      </c>
+      <c r="D18" s="6">
+        <v>2</v>
+      </c>
+      <c r="E18" s="18">
+        <v>44732</v>
+      </c>
+      <c r="F18" s="18">
+        <v>44739</v>
+      </c>
+      <c r="G18" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="11">
-        <v>70200000002</v>
-      </c>
-      <c r="I5" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" s="12">
-        <v>36911</v>
-      </c>
-      <c r="K5" s="11">
-        <v>0</v>
-      </c>
-      <c r="L5" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="M5" s="11">
-        <v>0</v>
-      </c>
-      <c r="N5" s="11">
-        <v>1</v>
-      </c>
-      <c r="O5" s="11">
-        <v>0</v>
-      </c>
-      <c r="P5" s="11">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11">
-        <v>4</v>
-      </c>
-      <c r="B6" s="11">
-        <v>2</v>
-      </c>
-      <c r="C6" s="11">
-        <v>3</v>
-      </c>
-      <c r="D6" s="11">
-        <v>2</v>
-      </c>
-      <c r="E6" s="12">
-        <v>44728</v>
-      </c>
-      <c r="F6" s="12">
-        <v>44863</v>
-      </c>
-      <c r="G6" s="11" t="s">
+      <c r="H18" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="J18" s="7">
+        <v>36810</v>
+      </c>
+      <c r="K18" s="6">
+        <v>0</v>
+      </c>
+      <c r="L18" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="11">
-        <v>70200000003</v>
-      </c>
-      <c r="I6" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="J6" s="12">
-        <v>37230</v>
-      </c>
-      <c r="K6" s="11">
-        <v>1</v>
-      </c>
-      <c r="L6" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M6" s="11">
-        <v>1</v>
-      </c>
-      <c r="N6" s="11">
-        <v>0</v>
-      </c>
-      <c r="O6" s="11">
-        <v>1</v>
-      </c>
-      <c r="P6" s="11">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11">
-        <v>5</v>
-      </c>
-      <c r="B7" s="11">
-        <v>4</v>
-      </c>
-      <c r="C7" s="11">
-        <v>1</v>
-      </c>
-      <c r="D7" s="11">
-        <v>2</v>
-      </c>
-      <c r="E7" s="12">
-        <v>44730</v>
-      </c>
-      <c r="F7" s="12">
-        <v>44926</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="11">
-        <v>70200000004</v>
-      </c>
-      <c r="I7" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="J7" s="12">
-        <v>37010</v>
-      </c>
-      <c r="K7" s="11">
-        <v>0</v>
-      </c>
-      <c r="L7" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="M7" s="11">
-        <v>0</v>
-      </c>
-      <c r="N7" s="11">
-        <v>1</v>
-      </c>
-      <c r="O7" s="11">
-        <v>0</v>
-      </c>
-      <c r="P7" s="11">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11">
-        <v>6</v>
-      </c>
-      <c r="B8" s="11">
-        <v>2</v>
-      </c>
-      <c r="C8" s="11">
-        <v>2</v>
-      </c>
-      <c r="D8" s="11">
-        <v>2</v>
-      </c>
-      <c r="E8" s="12">
-        <v>44732</v>
-      </c>
-      <c r="F8" s="12">
-        <v>44989</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="11">
-        <v>70200000005</v>
-      </c>
-      <c r="I8" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="J8" s="12">
-        <v>36790</v>
-      </c>
-      <c r="K8" s="11">
-        <v>1</v>
-      </c>
-      <c r="L8" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M8" s="11">
-        <v>1</v>
-      </c>
-      <c r="N8" s="11">
-        <v>0</v>
-      </c>
-      <c r="O8" s="11">
-        <v>1</v>
-      </c>
-      <c r="P8" s="11">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11">
-        <v>7</v>
-      </c>
-      <c r="B9" s="11">
-        <v>2</v>
-      </c>
-      <c r="C9" s="11">
-        <v>2</v>
-      </c>
-      <c r="D9" s="11">
-        <v>1</v>
-      </c>
-      <c r="E9" s="12">
-        <v>44734</v>
-      </c>
-      <c r="F9" s="12">
-        <v>45052</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="11">
-        <v>70200000006</v>
-      </c>
-      <c r="I9" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="J9" s="12">
-        <v>36570</v>
-      </c>
-      <c r="K9" s="11">
-        <v>0</v>
-      </c>
-      <c r="L9" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="M9" s="11">
-        <v>0</v>
-      </c>
-      <c r="N9" s="11">
-        <v>1</v>
-      </c>
-      <c r="O9" s="11">
-        <v>1</v>
-      </c>
-      <c r="P9" s="11">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11">
-        <v>8</v>
-      </c>
-      <c r="B10" s="11">
-        <v>1</v>
-      </c>
-      <c r="C10" s="11">
-        <v>1</v>
-      </c>
-      <c r="D10" s="11">
-        <v>2</v>
-      </c>
-      <c r="E10" s="12">
-        <v>44736</v>
-      </c>
-      <c r="F10" s="12">
-        <v>45115</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" s="11">
-        <v>70200000007</v>
-      </c>
-      <c r="I10" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="J10" s="12">
-        <v>36350</v>
-      </c>
-      <c r="K10" s="11">
-        <v>1</v>
-      </c>
-      <c r="L10" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M10" s="11">
-        <v>0</v>
-      </c>
-      <c r="N10" s="11">
-        <v>1</v>
-      </c>
-      <c r="O10" s="11">
-        <v>0</v>
-      </c>
-      <c r="P10" s="11">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11">
-        <v>9</v>
-      </c>
-      <c r="B11" s="11">
-        <v>3</v>
-      </c>
-      <c r="C11" s="11">
-        <v>3</v>
-      </c>
-      <c r="D11" s="11">
-        <v>2</v>
-      </c>
-      <c r="E11" s="12">
-        <v>44738</v>
-      </c>
-      <c r="F11" s="12">
-        <v>45178</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11" s="11">
-        <v>70200000008</v>
-      </c>
-      <c r="I11" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J11" s="12">
-        <v>36130</v>
-      </c>
-      <c r="K11" s="11">
-        <v>0</v>
-      </c>
-      <c r="L11" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="M11" s="11">
-        <v>1</v>
-      </c>
-      <c r="N11" s="11">
-        <v>0</v>
-      </c>
-      <c r="O11" s="11">
-        <v>1</v>
-      </c>
-      <c r="P11" s="11">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11">
-        <v>10</v>
-      </c>
-      <c r="B12" s="11">
-        <v>2</v>
-      </c>
-      <c r="C12" s="11">
-        <v>1</v>
-      </c>
-      <c r="D12" s="11">
-        <v>2</v>
-      </c>
-      <c r="E12" s="12">
-        <v>44740</v>
-      </c>
-      <c r="F12" s="12">
-        <v>45241</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" s="11">
-        <v>70200000009</v>
-      </c>
-      <c r="I12" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="J12" s="12">
-        <v>35910</v>
-      </c>
-      <c r="K12" s="11">
-        <v>1</v>
-      </c>
-      <c r="L12" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M12" s="11">
-        <v>0</v>
-      </c>
-      <c r="N12" s="11">
-        <v>0</v>
-      </c>
-      <c r="O12" s="11">
-        <v>1</v>
-      </c>
-      <c r="P12" s="11">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11">
-        <v>11</v>
-      </c>
-      <c r="B13" s="11">
-        <v>4</v>
-      </c>
-      <c r="C13" s="11">
-        <v>1</v>
-      </c>
-      <c r="D13" s="11">
-        <v>2</v>
-      </c>
-      <c r="E13" s="12">
-        <v>44742</v>
-      </c>
-      <c r="F13" s="12">
-        <v>45304</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H13" s="11">
-        <v>70200000010</v>
-      </c>
-      <c r="I13" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="J13" s="12">
-        <v>35690</v>
-      </c>
-      <c r="K13" s="11">
-        <v>0</v>
-      </c>
-      <c r="L13" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="M13" s="11">
-        <v>0</v>
-      </c>
-      <c r="N13" s="11">
-        <v>1</v>
-      </c>
-      <c r="O13" s="11">
-        <v>0</v>
-      </c>
-      <c r="P13" s="11">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="11">
-        <v>12</v>
-      </c>
-      <c r="B14" s="11">
-        <v>2</v>
-      </c>
-      <c r="C14" s="11">
-        <v>1</v>
-      </c>
-      <c r="D14" s="11">
-        <v>2</v>
-      </c>
-      <c r="E14" s="12">
-        <v>44744</v>
-      </c>
-      <c r="F14" s="12">
-        <v>45367</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="H14" s="11">
-        <v>70200000011</v>
-      </c>
-      <c r="I14" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="J14" s="12">
-        <v>35470</v>
-      </c>
-      <c r="K14" s="11">
-        <v>1</v>
-      </c>
-      <c r="L14" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M14" s="11">
-        <v>1</v>
-      </c>
-      <c r="N14" s="11">
-        <v>1</v>
-      </c>
-      <c r="O14" s="11">
-        <v>0</v>
-      </c>
-      <c r="P14" s="11">
-        <v>1</v>
-      </c>
-      <c r="Q14" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="11">
-        <v>13</v>
-      </c>
-      <c r="B15" s="11">
-        <v>1</v>
-      </c>
-      <c r="C15" s="11">
-        <v>2</v>
-      </c>
-      <c r="D15" s="11">
-        <v>2</v>
-      </c>
-      <c r="E15" s="12">
-        <v>44746</v>
-      </c>
-      <c r="F15" s="12">
-        <v>45430</v>
-      </c>
-      <c r="G15" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H15" s="11">
-        <v>70200000012</v>
-      </c>
-      <c r="I15" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="J15" s="12">
-        <v>35250</v>
-      </c>
-      <c r="K15" s="11">
-        <v>1</v>
-      </c>
-      <c r="L15" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="M15" s="11">
-        <v>0</v>
-      </c>
-      <c r="N15" s="11">
-        <v>1</v>
-      </c>
-      <c r="O15" s="11">
-        <v>0</v>
-      </c>
-      <c r="P15" s="11">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="11">
-        <v>14</v>
-      </c>
-      <c r="B16" s="11">
-        <v>3</v>
-      </c>
-      <c r="C16" s="11">
-        <v>2</v>
-      </c>
-      <c r="D16" s="11">
-        <v>2</v>
-      </c>
-      <c r="E16" s="12">
-        <v>44748</v>
-      </c>
-      <c r="F16" s="12">
-        <v>45493</v>
-      </c>
-      <c r="G16" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="H16" s="11">
-        <v>70200000013</v>
-      </c>
-      <c r="I16" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="J16" s="12">
-        <v>35030</v>
-      </c>
-      <c r="K16" s="11">
-        <v>1</v>
-      </c>
-      <c r="L16" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M16" s="11">
-        <v>1</v>
-      </c>
-      <c r="N16" s="11">
-        <v>0</v>
-      </c>
-      <c r="O16" s="11">
-        <v>0</v>
-      </c>
-      <c r="P16" s="11">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="11">
-        <v>15</v>
-      </c>
-      <c r="B17" s="11">
-        <v>2</v>
-      </c>
-      <c r="C17" s="11">
-        <v>1</v>
-      </c>
-      <c r="D17" s="11">
-        <v>2</v>
-      </c>
-      <c r="E17" s="12">
-        <v>44750</v>
-      </c>
-      <c r="F17" s="12">
-        <v>45556</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H17" s="11">
-        <v>70200000014</v>
-      </c>
-      <c r="I17" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="J17" s="12">
-        <v>34810</v>
-      </c>
-      <c r="K17" s="11">
-        <v>0</v>
-      </c>
-      <c r="L17" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="M17" s="11">
-        <v>0</v>
-      </c>
-      <c r="N17" s="11">
-        <v>0</v>
-      </c>
-      <c r="O17" s="11">
-        <v>0</v>
-      </c>
-      <c r="P17" s="11">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="11">
+      <c r="M18" s="6">
+        <v>0</v>
+      </c>
+      <c r="N18" s="6">
+        <v>0</v>
+      </c>
+      <c r="O18" s="6">
+        <v>0</v>
+      </c>
+      <c r="P18" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="6">
         <v>0</v>
       </c>
     </row>
@@ -2784,16 +2942,22 @@
     <mergeCell ref="G1:L1"/>
     <mergeCell ref="M1:Q1"/>
   </mergeCells>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="I3:I9" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B840CFF8BCBCC04B9FBF78A2B37C603B" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f8c3b211f390d76d2b813cea105395d2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="45e2578b-5781-47e1-85a2-a2bca000d7fe" xmlns:ns4="23dced98-c23c-4266-be03-749ab8bb2b21" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fdb726b0246e884b034b5f8cf6d0c271" ns3:_="" ns4:_="">
     <xsd:import namespace="45e2578b-5781-47e1-85a2-a2bca000d7fe"/>
@@ -3002,22 +3166,21 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8E843C9-AFC0-407A-892D-C6431DD2F37F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{937FC52D-6EB8-4763-9B21-6D5B28467E89}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3036,7 +3199,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D6B5C1E-8E64-4C3F-8B9C-ADE9CAA17D4A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -3051,12 +3214,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8E843C9-AFC0-407A-892D-C6431DD2F37F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Baseline funcion order room with import file
</commit_message>
<xml_diff>
--- a/SEP-VanLangHotel/Upload/Demo.xlsx
+++ b/SEP-VanLangHotel/Upload/Demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dangt\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2053B517-0FFA-4F0B-B744-7CB3A3C01A7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E77D321B-9CFC-4EB2-B861-AAA05B09DFC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{E93DE5FD-DC7B-498D-86AD-F192523F8D5C}"/>
   </bookViews>
@@ -1268,8 +1268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{109A43A6-863B-46FC-9A23-A5E8CB888B4E}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1984,8 +1984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1EC22DE-93F5-4706-915E-304A5F11A983}">
   <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add function empty rooms management
</commit_message>
<xml_diff>
--- a/SEP-VanLangHotel/Upload/Demo.xlsx
+++ b/SEP-VanLangHotel/Upload/Demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dangt\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32D0CFA-011E-4328-B581-70E513240210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5967A96A-6857-4760-9B02-C2C7490763E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="595" xr2:uid="{E93DE5FD-DC7B-498D-86AD-F192523F8D5C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="125">
   <si>
     <t>STT</t>
   </si>
@@ -132,16 +132,10 @@
 Nữ (0)</t>
   </si>
   <si>
-    <t>Nếu số người lớn &lt;= 2 và trẻ em &lt;= 2</t>
-  </si>
-  <si>
     <t>Nếu số người lớn = 3 người lớn và trẻ em &lt;= 3</t>
   </si>
   <si>
     <t>Nếu số người lớn = 4 người lớn và trẻ em &lt;= 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nếu số người lớn &lt;= 2 và trẻ em từ &lt;= 4 </t>
   </si>
   <si>
     <t>Ngày sinh (Năm-Tháng-Ngày)
@@ -857,6 +851,29 @@
   <si>
     <t>4F</t>
   </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>2
+1</t>
+  </si>
+  <si>
+    <t>2
+3</t>
+  </si>
+  <si>
+    <t>Nếu số người lớn = 2 và trẻ em &lt;= 2
+Nếu số người lớn = 1 và trẻ em &lt;= 3</t>
+  </si>
+  <si>
+    <t>4
+5</t>
+  </si>
+  <si>
+    <t>Nếu số người lớn = 2 và trẻ em từ &lt;= 4 
+Nếu số người lớn = 1 và trẻ em từ &lt;= 5</t>
+  </si>
 </sst>
 </file>
 
@@ -865,12 +882,20 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1508,17 +1533,17 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1560,91 +1585,79 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1656,46 +1669,67 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1749,86 +1783,92 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2148,7 +2188,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2162,53 +2202,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="61" t="s">
+      <c r="C1" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="61" t="s">
+      <c r="D1" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="61" t="s">
+      <c r="E1" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="63" t="s">
+      <c r="F1" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="55" t="s">
+      <c r="G1" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="57" t="s">
+      <c r="H1" s="60" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="60"/>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="58"/>
-    </row>
-    <row r="3" spans="1:8" ht="22.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="103" t="s">
-        <v>97</v>
+      <c r="A2" s="63"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="61"/>
+    </row>
+    <row r="3" spans="1:8" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="48" t="s">
+        <v>95</v>
       </c>
       <c r="B3" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="27">
-        <v>2</v>
-      </c>
-      <c r="D3" s="27">
-        <v>2</v>
+      <c r="C3" s="106" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3" s="106" t="s">
+        <v>121</v>
       </c>
       <c r="E3" s="27">
         <v>1</v>
@@ -2216,25 +2256,25 @@
       <c r="F3" s="28">
         <v>250000</v>
       </c>
-      <c r="G3" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="H3" s="52" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="22.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="103" t="s">
-        <v>98</v>
+      <c r="G3" s="107" t="s">
+        <v>122</v>
+      </c>
+      <c r="H3" s="55" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="31.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="48" t="s">
+        <v>96</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="1">
-        <v>2</v>
-      </c>
-      <c r="D4" s="1">
-        <v>4</v>
+      <c r="C4" s="110" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" s="110" t="s">
+        <v>123</v>
       </c>
       <c r="E4" s="1">
         <v>2</v>
@@ -2242,14 +2282,14 @@
       <c r="F4" s="2">
         <v>400000</v>
       </c>
-      <c r="G4" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" s="53"/>
+      <c r="G4" s="111" t="s">
+        <v>124</v>
+      </c>
+      <c r="H4" s="56"/>
     </row>
     <row r="5" spans="1:8" ht="22.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="103" t="s">
-        <v>99</v>
+      <c r="A5" s="48" t="s">
+        <v>97</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>21</v>
@@ -2266,143 +2306,143 @@
       <c r="F5" s="2">
         <v>500000</v>
       </c>
-      <c r="G5" s="31" t="s">
+      <c r="G5" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="56"/>
+    </row>
+    <row r="6" spans="1:8" ht="22.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="48" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="30">
+        <v>4</v>
+      </c>
+      <c r="D6" s="30">
+        <v>2</v>
+      </c>
+      <c r="E6" s="30">
+        <v>2</v>
+      </c>
+      <c r="F6" s="31">
+        <v>600000</v>
+      </c>
+      <c r="G6" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="53"/>
-    </row>
-    <row r="6" spans="1:8" ht="22.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="103" t="s">
+      <c r="H6" s="56"/>
+    </row>
+    <row r="7" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="109" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7" s="109" t="s">
+        <v>121</v>
+      </c>
+      <c r="E7" s="33">
+        <v>1</v>
+      </c>
+      <c r="F7" s="34">
+        <v>280000</v>
+      </c>
+      <c r="G7" s="108" t="s">
+        <v>122</v>
+      </c>
+      <c r="H7" s="56"/>
+    </row>
+    <row r="8" spans="1:8" ht="31.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="50" t="s">
         <v>100</v>
       </c>
-      <c r="B6" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="32">
+      <c r="B8" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="113" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8" s="113" t="s">
+        <v>123</v>
+      </c>
+      <c r="E8" s="35">
+        <v>2</v>
+      </c>
+      <c r="F8" s="36">
+        <v>430000</v>
+      </c>
+      <c r="G8" s="112" t="s">
+        <v>124</v>
+      </c>
+      <c r="H8" s="56"/>
+    </row>
+    <row r="9" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="B9" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="35">
+        <v>3</v>
+      </c>
+      <c r="D9" s="35">
+        <v>3</v>
+      </c>
+      <c r="E9" s="35">
+        <v>2</v>
+      </c>
+      <c r="F9" s="36">
+        <v>530000</v>
+      </c>
+      <c r="G9" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="56"/>
+    </row>
+    <row r="10" spans="1:8" ht="22.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="51" t="s">
+        <v>102</v>
+      </c>
+      <c r="B10" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="38">
         <v>4</v>
       </c>
-      <c r="D6" s="32">
+      <c r="D10" s="38">
         <v>2</v>
       </c>
-      <c r="E6" s="32">
+      <c r="E10" s="38">
         <v>2</v>
       </c>
-      <c r="F6" s="33">
-        <v>600000</v>
-      </c>
-      <c r="G6" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" s="53"/>
-    </row>
-    <row r="7" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="104" t="s">
-        <v>101</v>
-      </c>
-      <c r="B7" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="35">
-        <v>2</v>
-      </c>
-      <c r="D7" s="35">
-        <v>2</v>
-      </c>
-      <c r="E7" s="35">
-        <v>1</v>
-      </c>
-      <c r="F7" s="36">
-        <v>280000</v>
-      </c>
-      <c r="G7" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="H7" s="53"/>
-    </row>
-    <row r="8" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="105" t="s">
-        <v>102</v>
-      </c>
-      <c r="B8" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="38">
-        <v>2</v>
-      </c>
-      <c r="D8" s="38">
-        <v>4</v>
-      </c>
-      <c r="E8" s="38">
-        <v>2</v>
-      </c>
-      <c r="F8" s="39">
-        <v>430000</v>
-      </c>
-      <c r="G8" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="H8" s="53"/>
-    </row>
-    <row r="9" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="105" t="s">
+      <c r="F10" s="39">
+        <v>630000</v>
+      </c>
+      <c r="G10" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="57"/>
+    </row>
+    <row r="11" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="48" t="s">
         <v>103</v>
-      </c>
-      <c r="B9" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="38">
-        <v>3</v>
-      </c>
-      <c r="D9" s="38">
-        <v>3</v>
-      </c>
-      <c r="E9" s="38">
-        <v>2</v>
-      </c>
-      <c r="F9" s="39">
-        <v>530000</v>
-      </c>
-      <c r="G9" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="H9" s="53"/>
-    </row>
-    <row r="10" spans="1:8" ht="22.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="106" t="s">
-        <v>104</v>
-      </c>
-      <c r="B10" s="42" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="42">
-        <v>4</v>
-      </c>
-      <c r="D10" s="42">
-        <v>2</v>
-      </c>
-      <c r="E10" s="42">
-        <v>2</v>
-      </c>
-      <c r="F10" s="43">
-        <v>630000</v>
-      </c>
-      <c r="G10" s="44" t="s">
-        <v>33</v>
-      </c>
-      <c r="H10" s="54"/>
-    </row>
-    <row r="11" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="103" t="s">
-        <v>105</v>
       </c>
       <c r="B11" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="27">
-        <v>2</v>
-      </c>
-      <c r="D11" s="27">
-        <v>2</v>
+      <c r="C11" s="106" t="s">
+        <v>120</v>
+      </c>
+      <c r="D11" s="106" t="s">
+        <v>121</v>
       </c>
       <c r="E11" s="27">
         <v>1</v>
@@ -2410,23 +2450,23 @@
       <c r="F11" s="28">
         <v>310000</v>
       </c>
-      <c r="G11" s="29" t="s">
-        <v>31</v>
+      <c r="G11" s="107" t="s">
+        <v>122</v>
       </c>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="107" t="s">
-        <v>106</v>
+    <row r="12" spans="1:8" ht="31.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="52" t="s">
+        <v>104</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="1">
-        <v>2</v>
-      </c>
-      <c r="D12" s="1">
-        <v>4</v>
+      <c r="C12" s="110" t="s">
+        <v>120</v>
+      </c>
+      <c r="D12" s="110" t="s">
+        <v>123</v>
       </c>
       <c r="E12" s="1">
         <v>2</v>
@@ -2434,14 +2474,14 @@
       <c r="F12" s="2">
         <v>460000</v>
       </c>
-      <c r="G12" s="30" t="s">
-        <v>34</v>
+      <c r="G12" s="111" t="s">
+        <v>124</v>
       </c>
       <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="107" t="s">
-        <v>107</v>
+      <c r="A13" s="52" t="s">
+        <v>105</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>19</v>
@@ -2458,143 +2498,145 @@
       <c r="F13" s="2">
         <v>560000</v>
       </c>
-      <c r="G13" s="31" t="s">
+      <c r="G13" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="H13" s="54" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="22.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="53" t="s">
+        <v>106</v>
+      </c>
+      <c r="B14" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="30">
+        <v>4</v>
+      </c>
+      <c r="D14" s="30">
+        <v>2</v>
+      </c>
+      <c r="E14" s="30">
+        <v>2</v>
+      </c>
+      <c r="F14" s="31">
+        <v>660000</v>
+      </c>
+      <c r="G14" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="H13" s="3"/>
-    </row>
-    <row r="14" spans="1:8" ht="22.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="108" t="s">
+      <c r="H14" s="3"/>
+    </row>
+    <row r="15" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="49" t="s">
+        <v>107</v>
+      </c>
+      <c r="B15" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="109" t="s">
+        <v>120</v>
+      </c>
+      <c r="D15" s="109" t="s">
+        <v>121</v>
+      </c>
+      <c r="E15" s="33">
+        <v>1</v>
+      </c>
+      <c r="F15" s="34">
+        <v>340000</v>
+      </c>
+      <c r="G15" s="108" t="s">
+        <v>122</v>
+      </c>
+      <c r="H15" s="3"/>
+    </row>
+    <row r="16" spans="1:8" ht="31.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="50" t="s">
         <v>108</v>
       </c>
-      <c r="B14" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="32">
+      <c r="B16" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="113" t="s">
+        <v>120</v>
+      </c>
+      <c r="D16" s="113" t="s">
+        <v>123</v>
+      </c>
+      <c r="E16" s="35">
+        <v>2</v>
+      </c>
+      <c r="F16" s="36">
+        <v>490000</v>
+      </c>
+      <c r="G16" s="112" t="s">
+        <v>124</v>
+      </c>
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="50" t="s">
+        <v>109</v>
+      </c>
+      <c r="B17" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="35">
+        <v>3</v>
+      </c>
+      <c r="D17" s="35">
+        <v>3</v>
+      </c>
+      <c r="E17" s="35">
+        <v>2</v>
+      </c>
+      <c r="F17" s="36">
+        <v>590000</v>
+      </c>
+      <c r="G17" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="1:8" ht="22.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="51" t="s">
+        <v>110</v>
+      </c>
+      <c r="B18" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="38">
         <v>4</v>
       </c>
-      <c r="D14" s="32">
+      <c r="D18" s="38">
         <v>2</v>
       </c>
-      <c r="E14" s="32">
+      <c r="E18" s="38">
         <v>2</v>
       </c>
-      <c r="F14" s="33">
-        <v>660000</v>
-      </c>
-      <c r="G14" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="H14" s="3"/>
-    </row>
-    <row r="15" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="104" t="s">
-        <v>109</v>
-      </c>
-      <c r="B15" s="35" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="35">
-        <v>2</v>
-      </c>
-      <c r="D15" s="35">
-        <v>2</v>
-      </c>
-      <c r="E15" s="35">
-        <v>1</v>
-      </c>
-      <c r="F15" s="36">
-        <v>340000</v>
-      </c>
-      <c r="G15" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="H15" s="3"/>
-    </row>
-    <row r="16" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="105" t="s">
-        <v>110</v>
-      </c>
-      <c r="B16" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="38">
-        <v>2</v>
-      </c>
-      <c r="D16" s="38">
-        <v>4</v>
-      </c>
-      <c r="E16" s="38">
-        <v>2</v>
-      </c>
-      <c r="F16" s="39">
-        <v>490000</v>
-      </c>
-      <c r="G16" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="H16" s="3"/>
-    </row>
-    <row r="17" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="105" t="s">
+      <c r="F18" s="39">
+        <v>690000</v>
+      </c>
+      <c r="G18" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="48" t="s">
         <v>111</v>
-      </c>
-      <c r="B17" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="38">
-        <v>3</v>
-      </c>
-      <c r="D17" s="38">
-        <v>3</v>
-      </c>
-      <c r="E17" s="38">
-        <v>2</v>
-      </c>
-      <c r="F17" s="39">
-        <v>590000</v>
-      </c>
-      <c r="G17" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="H17" s="3"/>
-    </row>
-    <row r="18" spans="1:8" ht="22.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="106" t="s">
-        <v>112</v>
-      </c>
-      <c r="B18" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="42">
-        <v>4</v>
-      </c>
-      <c r="D18" s="42">
-        <v>2</v>
-      </c>
-      <c r="E18" s="42">
-        <v>2</v>
-      </c>
-      <c r="F18" s="43">
-        <v>690000</v>
-      </c>
-      <c r="G18" s="44" t="s">
-        <v>33</v>
-      </c>
-      <c r="H18" s="3"/>
-    </row>
-    <row r="19" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="103" t="s">
-        <v>113</v>
       </c>
       <c r="B19" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="27">
-        <v>2</v>
-      </c>
-      <c r="D19" s="27">
-        <v>2</v>
+      <c r="C19" s="106" t="s">
+        <v>120</v>
+      </c>
+      <c r="D19" s="106" t="s">
+        <v>121</v>
       </c>
       <c r="E19" s="27">
         <v>1</v>
@@ -2602,23 +2644,23 @@
       <c r="F19" s="28">
         <v>370000</v>
       </c>
-      <c r="G19" s="29" t="s">
-        <v>31</v>
+      <c r="G19" s="107" t="s">
+        <v>122</v>
       </c>
       <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="107" t="s">
-        <v>114</v>
+    <row r="20" spans="1:8" ht="31.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="52" t="s">
+        <v>112</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="1">
-        <v>2</v>
-      </c>
-      <c r="D20" s="1">
-        <v>4</v>
+      <c r="C20" s="110" t="s">
+        <v>120</v>
+      </c>
+      <c r="D20" s="110" t="s">
+        <v>123</v>
       </c>
       <c r="E20" s="1">
         <v>2</v>
@@ -2626,14 +2668,14 @@
       <c r="F20" s="2">
         <v>520000</v>
       </c>
-      <c r="G20" s="30" t="s">
-        <v>34</v>
+      <c r="G20" s="111" t="s">
+        <v>124</v>
       </c>
       <c r="H20" s="3"/>
     </row>
     <row r="21" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="107" t="s">
-        <v>115</v>
+      <c r="A21" s="52" t="s">
+        <v>113</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>17</v>
@@ -2650,128 +2692,128 @@
       <c r="F21" s="2">
         <v>620000</v>
       </c>
-      <c r="G21" s="31" t="s">
+      <c r="G21" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="H21" s="3"/>
+    </row>
+    <row r="22" spans="1:8" ht="22.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="53" t="s">
+        <v>114</v>
+      </c>
+      <c r="B22" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="30">
+        <v>4</v>
+      </c>
+      <c r="D22" s="30">
+        <v>2</v>
+      </c>
+      <c r="E22" s="30">
+        <v>2</v>
+      </c>
+      <c r="F22" s="31">
+        <v>720000</v>
+      </c>
+      <c r="G22" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="H21" s="3"/>
-    </row>
-    <row r="22" spans="1:8" ht="22.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="108" t="s">
+      <c r="H22" s="3"/>
+    </row>
+    <row r="23" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="49" t="s">
+        <v>115</v>
+      </c>
+      <c r="B23" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="109" t="s">
+        <v>120</v>
+      </c>
+      <c r="D23" s="109" t="s">
+        <v>121</v>
+      </c>
+      <c r="E23" s="33">
+        <v>1</v>
+      </c>
+      <c r="F23" s="34">
+        <v>220000</v>
+      </c>
+      <c r="G23" s="108" t="s">
+        <v>122</v>
+      </c>
+      <c r="H23" s="3"/>
+    </row>
+    <row r="24" spans="1:8" ht="31.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="50" t="s">
         <v>116</v>
       </c>
-      <c r="B22" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" s="32">
+      <c r="B24" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="113" t="s">
+        <v>120</v>
+      </c>
+      <c r="D24" s="113" t="s">
+        <v>123</v>
+      </c>
+      <c r="E24" s="35">
+        <v>2</v>
+      </c>
+      <c r="F24" s="36">
+        <v>370000</v>
+      </c>
+      <c r="G24" s="112" t="s">
+        <v>124</v>
+      </c>
+      <c r="H24" s="3"/>
+    </row>
+    <row r="25" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="50" t="s">
+        <v>117</v>
+      </c>
+      <c r="B25" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="35">
+        <v>3</v>
+      </c>
+      <c r="D25" s="35">
+        <v>3</v>
+      </c>
+      <c r="E25" s="35">
+        <v>2</v>
+      </c>
+      <c r="F25" s="36">
+        <v>470000</v>
+      </c>
+      <c r="G25" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="H25" s="3"/>
+    </row>
+    <row r="26" spans="1:8" ht="22.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="51" t="s">
+        <v>118</v>
+      </c>
+      <c r="B26" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" s="38">
         <v>4</v>
       </c>
-      <c r="D22" s="32">
+      <c r="D26" s="38">
         <v>2</v>
       </c>
-      <c r="E22" s="32">
+      <c r="E26" s="38">
         <v>2</v>
       </c>
-      <c r="F22" s="33">
-        <v>720000</v>
-      </c>
-      <c r="G22" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="H22" s="3"/>
-    </row>
-    <row r="23" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="104" t="s">
-        <v>117</v>
-      </c>
-      <c r="B23" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="C23" s="35">
-        <v>2</v>
-      </c>
-      <c r="D23" s="35">
-        <v>2</v>
-      </c>
-      <c r="E23" s="35">
-        <v>1</v>
-      </c>
-      <c r="F23" s="36">
-        <v>220000</v>
-      </c>
-      <c r="G23" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="H23" s="3"/>
-    </row>
-    <row r="24" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="105" t="s">
-        <v>118</v>
-      </c>
-      <c r="B24" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="C24" s="38">
-        <v>2</v>
-      </c>
-      <c r="D24" s="38">
-        <v>4</v>
-      </c>
-      <c r="E24" s="38">
-        <v>2</v>
-      </c>
-      <c r="F24" s="39">
-        <v>370000</v>
-      </c>
-      <c r="G24" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="H24" s="3"/>
-    </row>
-    <row r="25" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="105" t="s">
-        <v>119</v>
-      </c>
-      <c r="B25" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="C25" s="38">
-        <v>3</v>
-      </c>
-      <c r="D25" s="38">
-        <v>3</v>
-      </c>
-      <c r="E25" s="38">
-        <v>2</v>
-      </c>
-      <c r="F25" s="39">
-        <v>470000</v>
-      </c>
-      <c r="G25" s="41" t="s">
+      <c r="F26" s="39">
+        <v>570000</v>
+      </c>
+      <c r="G26" s="40" t="s">
         <v>32</v>
-      </c>
-      <c r="H25" s="3"/>
-    </row>
-    <row r="26" spans="1:8" ht="22.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="106" t="s">
-        <v>120</v>
-      </c>
-      <c r="B26" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="C26" s="42">
-        <v>4</v>
-      </c>
-      <c r="D26" s="42">
-        <v>2</v>
-      </c>
-      <c r="E26" s="42">
-        <v>2</v>
-      </c>
-      <c r="F26" s="43">
-        <v>570000</v>
-      </c>
-      <c r="G26" s="44" t="s">
-        <v>33</v>
       </c>
       <c r="H26" s="3"/>
     </row>
@@ -2787,7 +2829,7 @@
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
   </mergeCells>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2824,51 +2866,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="102" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="103"/>
+      <c r="C1" s="103"/>
+      <c r="D1" s="103"/>
+      <c r="E1" s="103"/>
+      <c r="F1" s="103"/>
+      <c r="G1" s="103"/>
+      <c r="H1" s="103"/>
+      <c r="I1" s="103"/>
+      <c r="J1" s="104"/>
+      <c r="K1" s="93" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" s="94"/>
+      <c r="M1" s="94"/>
+      <c r="N1" s="94"/>
+      <c r="O1" s="95"/>
+      <c r="P1" s="91" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q1" s="92"/>
+    </row>
+    <row r="2" spans="1:17" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="42" t="s">
         <v>90</v>
-      </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
-      <c r="I1" s="94"/>
-      <c r="J1" s="95"/>
-      <c r="K1" s="90" t="s">
-        <v>37</v>
-      </c>
-      <c r="L1" s="91"/>
-      <c r="M1" s="91"/>
-      <c r="N1" s="91"/>
-      <c r="O1" s="92"/>
-      <c r="P1" s="88" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q1" s="89"/>
-    </row>
-    <row r="2" spans="1:17" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="46" t="s">
-        <v>92</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="47" t="s">
-        <v>40</v>
+      <c r="C2" s="43" t="s">
+        <v>38</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="45" t="s">
+      <c r="F2" s="41" t="s">
         <v>4</v>
       </c>
       <c r="G2" s="21" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H2" s="21" t="s">
         <v>30</v>
@@ -2876,7 +2918,7 @@
       <c r="I2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="51" t="s">
+      <c r="J2" s="47" t="s">
         <v>1</v>
       </c>
       <c r="K2" s="25" t="s">
@@ -2895,27 +2937,27 @@
         <v>14</v>
       </c>
       <c r="P2" s="24" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="Q2" s="23" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="65">
+      <c r="A3" s="68">
         <v>1</v>
       </c>
       <c r="B3" s="16">
         <v>1</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="44" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="16"/>
       <c r="E3" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3" s="77" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="80" t="s">
         <v>5</v>
       </c>
       <c r="G3" s="11">
@@ -2925,46 +2967,46 @@
         <v>1</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="J3" s="68">
+        <v>41</v>
+      </c>
+      <c r="J3" s="71">
         <v>2</v>
       </c>
-      <c r="K3" s="71">
+      <c r="K3" s="74">
         <v>1</v>
       </c>
-      <c r="L3" s="74">
+      <c r="L3" s="77">
         <v>1</v>
       </c>
-      <c r="M3" s="74">
+      <c r="M3" s="77">
         <v>1</v>
       </c>
-      <c r="N3" s="74">
+      <c r="N3" s="77">
         <v>0</v>
       </c>
-      <c r="O3" s="68">
+      <c r="O3" s="71">
         <v>1</v>
       </c>
-      <c r="P3" s="82">
+      <c r="P3" s="85">
         <v>44765</v>
       </c>
-      <c r="Q3" s="85">
+      <c r="Q3" s="88">
         <v>44765</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="66"/>
+      <c r="A4" s="69"/>
       <c r="B4" s="17">
         <v>2</v>
       </c>
-      <c r="C4" s="49" t="s">
+      <c r="C4" s="45" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E4" s="7"/>
-      <c r="F4" s="78"/>
+      <c r="F4" s="81"/>
       <c r="G4" s="8">
         <v>39571</v>
       </c>
@@ -2972,30 +3014,30 @@
         <v>0</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="J4" s="69"/>
-      <c r="K4" s="72"/>
-      <c r="L4" s="75"/>
-      <c r="M4" s="75"/>
-      <c r="N4" s="75"/>
-      <c r="O4" s="69"/>
-      <c r="P4" s="83"/>
-      <c r="Q4" s="86"/>
+        <v>41</v>
+      </c>
+      <c r="J4" s="72"/>
+      <c r="K4" s="75"/>
+      <c r="L4" s="78"/>
+      <c r="M4" s="78"/>
+      <c r="N4" s="78"/>
+      <c r="O4" s="72"/>
+      <c r="P4" s="86"/>
+      <c r="Q4" s="89"/>
     </row>
     <row r="5" spans="1:17" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="66"/>
+      <c r="A5" s="69"/>
       <c r="B5" s="17">
         <v>3</v>
       </c>
-      <c r="C5" s="49" t="s">
+      <c r="C5" s="45" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E5" s="7"/>
-      <c r="F5" s="78"/>
+      <c r="F5" s="81"/>
       <c r="G5" s="8">
         <v>39459</v>
       </c>
@@ -3003,30 +3045,30 @@
         <v>1</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="J5" s="69"/>
-      <c r="K5" s="72"/>
-      <c r="L5" s="75"/>
-      <c r="M5" s="75"/>
-      <c r="N5" s="75"/>
-      <c r="O5" s="69"/>
-      <c r="P5" s="83"/>
-      <c r="Q5" s="86"/>
+        <v>41</v>
+      </c>
+      <c r="J5" s="72"/>
+      <c r="K5" s="75"/>
+      <c r="L5" s="78"/>
+      <c r="M5" s="78"/>
+      <c r="N5" s="78"/>
+      <c r="O5" s="72"/>
+      <c r="P5" s="86"/>
+      <c r="Q5" s="89"/>
     </row>
     <row r="6" spans="1:17" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="66"/>
+      <c r="A6" s="69"/>
       <c r="B6" s="17">
         <v>4</v>
       </c>
-      <c r="C6" s="49" t="s">
+      <c r="C6" s="45" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E6" s="7"/>
-      <c r="F6" s="78"/>
+      <c r="F6" s="81"/>
       <c r="G6" s="8">
         <v>40505</v>
       </c>
@@ -3034,30 +3076,30 @@
         <v>0</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="J6" s="69"/>
-      <c r="K6" s="72"/>
-      <c r="L6" s="75"/>
-      <c r="M6" s="75"/>
-      <c r="N6" s="75"/>
-      <c r="O6" s="69"/>
-      <c r="P6" s="83"/>
-      <c r="Q6" s="86"/>
+        <v>41</v>
+      </c>
+      <c r="J6" s="72"/>
+      <c r="K6" s="75"/>
+      <c r="L6" s="78"/>
+      <c r="M6" s="78"/>
+      <c r="N6" s="78"/>
+      <c r="O6" s="72"/>
+      <c r="P6" s="86"/>
+      <c r="Q6" s="89"/>
     </row>
     <row r="7" spans="1:17" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="67"/>
+      <c r="A7" s="70"/>
       <c r="B7" s="18">
         <v>5</v>
       </c>
-      <c r="C7" s="50" t="s">
+      <c r="C7" s="46" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E7" s="13"/>
-      <c r="F7" s="79"/>
+      <c r="F7" s="82"/>
       <c r="G7" s="14">
         <v>41149</v>
       </c>
@@ -3065,33 +3107,33 @@
         <v>0</v>
       </c>
       <c r="I7" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="J7" s="70"/>
-      <c r="K7" s="73"/>
-      <c r="L7" s="76"/>
-      <c r="M7" s="76"/>
-      <c r="N7" s="76"/>
-      <c r="O7" s="70"/>
-      <c r="P7" s="83"/>
-      <c r="Q7" s="86"/>
+        <v>41</v>
+      </c>
+      <c r="J7" s="73"/>
+      <c r="K7" s="76"/>
+      <c r="L7" s="79"/>
+      <c r="M7" s="79"/>
+      <c r="N7" s="79"/>
+      <c r="O7" s="73"/>
+      <c r="P7" s="86"/>
+      <c r="Q7" s="89"/>
     </row>
     <row r="8" spans="1:17" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A8" s="65">
+      <c r="A8" s="68">
         <v>2</v>
       </c>
       <c r="B8" s="16">
         <v>1</v>
       </c>
-      <c r="C8" s="48" t="s">
-        <v>44</v>
+      <c r="C8" s="44" t="s">
+        <v>42</v>
       </c>
       <c r="D8" s="16"/>
       <c r="E8" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="F8" s="77" t="s">
-        <v>96</v>
+        <v>48</v>
+      </c>
+      <c r="F8" s="80" t="s">
+        <v>94</v>
       </c>
       <c r="G8" s="11">
         <v>37157</v>
@@ -3100,44 +3142,44 @@
         <v>1</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="J8" s="68">
+        <v>85</v>
+      </c>
+      <c r="J8" s="71">
         <v>2</v>
       </c>
-      <c r="K8" s="71">
+      <c r="K8" s="74">
         <v>1</v>
       </c>
-      <c r="L8" s="74">
+      <c r="L8" s="77">
         <v>0</v>
       </c>
-      <c r="M8" s="74">
+      <c r="M8" s="77">
         <v>1</v>
       </c>
-      <c r="N8" s="74">
+      <c r="N8" s="77">
         <v>0</v>
       </c>
-      <c r="O8" s="68">
+      <c r="O8" s="71">
         <v>0</v>
       </c>
-      <c r="P8" s="83"/>
-      <c r="Q8" s="86"/>
+      <c r="P8" s="86"/>
+      <c r="Q8" s="89"/>
     </row>
     <row r="9" spans="1:17" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A9" s="66"/>
+      <c r="A9" s="69"/>
       <c r="B9" s="17">
         <v>2</v>
       </c>
-      <c r="C9" s="49" t="s">
-        <v>45</v>
+      <c r="C9" s="45" t="s">
+        <v>43</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="F9" s="78"/>
+        <v>61</v>
+      </c>
+      <c r="F9" s="81"/>
       <c r="G9" s="8">
         <v>36904</v>
       </c>
@@ -3145,32 +3187,32 @@
         <v>1</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="J9" s="69"/>
-      <c r="K9" s="72"/>
-      <c r="L9" s="75"/>
-      <c r="M9" s="75"/>
-      <c r="N9" s="75"/>
-      <c r="O9" s="69"/>
-      <c r="P9" s="83"/>
-      <c r="Q9" s="86"/>
+        <v>84</v>
+      </c>
+      <c r="J9" s="72"/>
+      <c r="K9" s="75"/>
+      <c r="L9" s="78"/>
+      <c r="M9" s="78"/>
+      <c r="N9" s="78"/>
+      <c r="O9" s="72"/>
+      <c r="P9" s="86"/>
+      <c r="Q9" s="89"/>
     </row>
     <row r="10" spans="1:17" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A10" s="66"/>
+      <c r="A10" s="69"/>
       <c r="B10" s="17">
         <v>3</v>
       </c>
-      <c r="C10" s="49" t="s">
-        <v>47</v>
+      <c r="C10" s="45" t="s">
+        <v>45</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F10" s="78"/>
+        <v>62</v>
+      </c>
+      <c r="F10" s="81"/>
       <c r="G10" s="8">
         <v>37004</v>
       </c>
@@ -3178,32 +3220,32 @@
         <v>0</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="J10" s="69"/>
-      <c r="K10" s="72"/>
-      <c r="L10" s="75"/>
-      <c r="M10" s="75"/>
-      <c r="N10" s="75"/>
-      <c r="O10" s="69"/>
-      <c r="P10" s="83"/>
-      <c r="Q10" s="86"/>
+        <v>83</v>
+      </c>
+      <c r="J10" s="72"/>
+      <c r="K10" s="75"/>
+      <c r="L10" s="78"/>
+      <c r="M10" s="78"/>
+      <c r="N10" s="78"/>
+      <c r="O10" s="72"/>
+      <c r="P10" s="86"/>
+      <c r="Q10" s="89"/>
     </row>
     <row r="11" spans="1:17" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A11" s="66"/>
+      <c r="A11" s="69"/>
       <c r="B11" s="17">
         <v>4</v>
       </c>
-      <c r="C11" s="49" t="s">
-        <v>48</v>
+      <c r="C11" s="45" t="s">
+        <v>46</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="F11" s="78"/>
+        <v>63</v>
+      </c>
+      <c r="F11" s="81"/>
       <c r="G11" s="8">
         <v>37210</v>
       </c>
@@ -3211,32 +3253,32 @@
         <v>0</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="J11" s="69"/>
-      <c r="K11" s="72"/>
-      <c r="L11" s="75"/>
-      <c r="M11" s="75"/>
-      <c r="N11" s="75"/>
-      <c r="O11" s="69"/>
-      <c r="P11" s="83"/>
-      <c r="Q11" s="86"/>
+        <v>82</v>
+      </c>
+      <c r="J11" s="72"/>
+      <c r="K11" s="75"/>
+      <c r="L11" s="78"/>
+      <c r="M11" s="78"/>
+      <c r="N11" s="78"/>
+      <c r="O11" s="72"/>
+      <c r="P11" s="86"/>
+      <c r="Q11" s="89"/>
     </row>
     <row r="12" spans="1:17" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="67"/>
+      <c r="A12" s="70"/>
       <c r="B12" s="18">
         <v>5</v>
       </c>
-      <c r="C12" s="50" t="s">
-        <v>49</v>
+      <c r="C12" s="46" t="s">
+        <v>47</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="F12" s="79"/>
+        <v>64</v>
+      </c>
+      <c r="F12" s="82"/>
       <c r="G12" s="14">
         <v>39500</v>
       </c>
@@ -3244,33 +3286,33 @@
         <v>0</v>
       </c>
       <c r="I12" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="J12" s="70"/>
-      <c r="K12" s="73"/>
-      <c r="L12" s="76"/>
-      <c r="M12" s="76"/>
-      <c r="N12" s="76"/>
-      <c r="O12" s="70"/>
-      <c r="P12" s="83"/>
-      <c r="Q12" s="86"/>
+        <v>81</v>
+      </c>
+      <c r="J12" s="73"/>
+      <c r="K12" s="76"/>
+      <c r="L12" s="79"/>
+      <c r="M12" s="79"/>
+      <c r="N12" s="79"/>
+      <c r="O12" s="73"/>
+      <c r="P12" s="86"/>
+      <c r="Q12" s="89"/>
     </row>
     <row r="13" spans="1:17" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A13" s="65">
+      <c r="A13" s="68">
         <v>3</v>
       </c>
       <c r="B13" s="16">
         <v>1</v>
       </c>
-      <c r="C13" s="48" t="s">
-        <v>55</v>
+      <c r="C13" s="44" t="s">
+        <v>53</v>
       </c>
       <c r="D13" s="16"/>
       <c r="E13" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="F13" s="77" t="s">
-        <v>53</v>
+        <v>34</v>
+      </c>
+      <c r="F13" s="80" t="s">
+        <v>51</v>
       </c>
       <c r="G13" s="11">
         <v>36965</v>
@@ -3279,12 +3321,12 @@
         <v>1</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="J13" s="68">
+        <v>80</v>
+      </c>
+      <c r="J13" s="71">
         <v>1</v>
       </c>
-      <c r="K13" s="80">
+      <c r="K13" s="83">
         <v>0</v>
       </c>
       <c r="L13" s="96">
@@ -3299,24 +3341,24 @@
       <c r="O13" s="98">
         <v>1</v>
       </c>
-      <c r="P13" s="83"/>
-      <c r="Q13" s="86"/>
+      <c r="P13" s="86"/>
+      <c r="Q13" s="89"/>
     </row>
     <row r="14" spans="1:17" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="67"/>
+      <c r="A14" s="70"/>
       <c r="B14" s="18">
         <v>2</v>
       </c>
-      <c r="C14" s="50" t="s">
-        <v>56</v>
+      <c r="C14" s="46" t="s">
+        <v>54</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="F14" s="79"/>
+        <v>59</v>
+      </c>
+      <c r="F14" s="82"/>
       <c r="G14" s="14">
         <v>37459</v>
       </c>
@@ -3324,33 +3366,33 @@
         <v>0</v>
       </c>
       <c r="I14" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="J14" s="70"/>
-      <c r="K14" s="81"/>
+        <v>60</v>
+      </c>
+      <c r="J14" s="73"/>
+      <c r="K14" s="84"/>
       <c r="L14" s="97"/>
       <c r="M14" s="97"/>
       <c r="N14" s="97"/>
       <c r="O14" s="99"/>
-      <c r="P14" s="83"/>
-      <c r="Q14" s="86"/>
+      <c r="P14" s="86"/>
+      <c r="Q14" s="89"/>
     </row>
     <row r="15" spans="1:17" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A15" s="65">
+      <c r="A15" s="68">
         <v>4</v>
       </c>
       <c r="B15" s="16">
         <v>1</v>
       </c>
-      <c r="C15" s="48" t="s">
-        <v>67</v>
+      <c r="C15" s="44" t="s">
+        <v>65</v>
       </c>
       <c r="D15" s="16"/>
       <c r="E15" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="F15" s="77" t="s">
-        <v>51</v>
+        <v>69</v>
+      </c>
+      <c r="F15" s="80" t="s">
+        <v>49</v>
       </c>
       <c r="G15" s="11">
         <v>36965</v>
@@ -3359,12 +3401,12 @@
         <v>1</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="J15" s="68">
+        <v>76</v>
+      </c>
+      <c r="J15" s="71">
         <v>2</v>
       </c>
-      <c r="K15" s="80">
+      <c r="K15" s="83">
         <v>0</v>
       </c>
       <c r="L15" s="96">
@@ -3379,24 +3421,24 @@
       <c r="O15" s="98">
         <v>1</v>
       </c>
-      <c r="P15" s="83"/>
-      <c r="Q15" s="86"/>
+      <c r="P15" s="86"/>
+      <c r="Q15" s="89"/>
     </row>
     <row r="16" spans="1:17" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A16" s="66"/>
+      <c r="A16" s="69"/>
       <c r="B16" s="17">
         <v>2</v>
       </c>
-      <c r="C16" s="49" t="s">
-        <v>68</v>
+      <c r="C16" s="45" t="s">
+        <v>66</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="F16" s="78"/>
+        <v>70</v>
+      </c>
+      <c r="F16" s="81"/>
       <c r="G16" s="8">
         <v>38555</v>
       </c>
@@ -3404,32 +3446,32 @@
         <v>1</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="J16" s="69"/>
+        <v>77</v>
+      </c>
+      <c r="J16" s="72"/>
       <c r="K16" s="100"/>
       <c r="L16" s="101"/>
       <c r="M16" s="101"/>
       <c r="N16" s="101"/>
-      <c r="O16" s="102"/>
-      <c r="P16" s="83"/>
-      <c r="Q16" s="86"/>
+      <c r="O16" s="105"/>
+      <c r="P16" s="86"/>
+      <c r="Q16" s="89"/>
     </row>
     <row r="17" spans="1:17" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A17" s="66"/>
+      <c r="A17" s="69"/>
       <c r="B17" s="17">
         <v>3</v>
       </c>
-      <c r="C17" s="49" t="s">
-        <v>69</v>
+      <c r="C17" s="45" t="s">
+        <v>67</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="F17" s="78"/>
+        <v>71</v>
+      </c>
+      <c r="F17" s="81"/>
       <c r="G17" s="8">
         <v>37667</v>
       </c>
@@ -3437,32 +3479,32 @@
         <v>1</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="J17" s="69"/>
+        <v>78</v>
+      </c>
+      <c r="J17" s="72"/>
       <c r="K17" s="100"/>
       <c r="L17" s="101"/>
       <c r="M17" s="101"/>
       <c r="N17" s="101"/>
-      <c r="O17" s="102"/>
-      <c r="P17" s="83"/>
-      <c r="Q17" s="86"/>
+      <c r="O17" s="105"/>
+      <c r="P17" s="86"/>
+      <c r="Q17" s="89"/>
     </row>
     <row r="18" spans="1:17" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="67"/>
+      <c r="A18" s="70"/>
       <c r="B18" s="18">
         <v>4</v>
       </c>
-      <c r="C18" s="50" t="s">
-        <v>70</v>
+      <c r="C18" s="46" t="s">
+        <v>68</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="F18" s="79"/>
+        <v>72</v>
+      </c>
+      <c r="F18" s="82"/>
       <c r="G18" s="14">
         <v>37485</v>
       </c>
@@ -3470,33 +3512,33 @@
         <v>1</v>
       </c>
       <c r="I18" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="J18" s="70"/>
-      <c r="K18" s="81"/>
+        <v>79</v>
+      </c>
+      <c r="J18" s="73"/>
+      <c r="K18" s="84"/>
       <c r="L18" s="97"/>
       <c r="M18" s="97"/>
       <c r="N18" s="97"/>
       <c r="O18" s="99"/>
-      <c r="P18" s="83"/>
-      <c r="Q18" s="86"/>
+      <c r="P18" s="86"/>
+      <c r="Q18" s="89"/>
     </row>
     <row r="19" spans="1:17" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A19" s="65">
+      <c r="A19" s="68">
         <v>5</v>
       </c>
       <c r="B19" s="16">
         <v>1</v>
       </c>
-      <c r="C19" s="48" t="s">
-        <v>57</v>
+      <c r="C19" s="44" t="s">
+        <v>55</v>
       </c>
       <c r="D19" s="16"/>
       <c r="E19" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F19" s="80" t="s">
         <v>52</v>
-      </c>
-      <c r="F19" s="77" t="s">
-        <v>54</v>
       </c>
       <c r="G19" s="11">
         <v>36965</v>
@@ -3505,12 +3547,12 @@
         <v>1</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="J19" s="68">
+        <v>75</v>
+      </c>
+      <c r="J19" s="71">
         <v>2</v>
       </c>
-      <c r="K19" s="80">
+      <c r="K19" s="83">
         <v>1</v>
       </c>
       <c r="L19" s="96">
@@ -3525,22 +3567,22 @@
       <c r="O19" s="98">
         <v>1</v>
       </c>
-      <c r="P19" s="83"/>
-      <c r="Q19" s="86"/>
+      <c r="P19" s="86"/>
+      <c r="Q19" s="89"/>
     </row>
     <row r="20" spans="1:17" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A20" s="66"/>
+      <c r="A20" s="69"/>
       <c r="B20" s="17">
         <v>2</v>
       </c>
-      <c r="C20" s="49" t="s">
-        <v>58</v>
+      <c r="C20" s="45" t="s">
+        <v>56</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E20" s="7"/>
-      <c r="F20" s="78"/>
+      <c r="F20" s="81"/>
       <c r="G20" s="8">
         <v>40016</v>
       </c>
@@ -3548,30 +3590,30 @@
         <v>1</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="J20" s="69"/>
+        <v>86</v>
+      </c>
+      <c r="J20" s="72"/>
       <c r="K20" s="100"/>
       <c r="L20" s="101"/>
       <c r="M20" s="101"/>
       <c r="N20" s="101"/>
-      <c r="O20" s="102"/>
-      <c r="P20" s="83"/>
-      <c r="Q20" s="86"/>
+      <c r="O20" s="105"/>
+      <c r="P20" s="86"/>
+      <c r="Q20" s="89"/>
     </row>
     <row r="21" spans="1:17" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="67"/>
+      <c r="A21" s="70"/>
       <c r="B21" s="18">
         <v>3</v>
       </c>
-      <c r="C21" s="50" t="s">
-        <v>59</v>
+      <c r="C21" s="46" t="s">
+        <v>57</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E21" s="13"/>
-      <c r="F21" s="79"/>
+      <c r="F21" s="82"/>
       <c r="G21" s="14">
         <v>40224</v>
       </c>
@@ -3579,16 +3621,16 @@
         <v>0</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="J21" s="70"/>
-      <c r="K21" s="81"/>
+        <v>87</v>
+      </c>
+      <c r="J21" s="73"/>
+      <c r="K21" s="84"/>
       <c r="L21" s="97"/>
       <c r="M21" s="97"/>
       <c r="N21" s="97"/>
       <c r="O21" s="99"/>
-      <c r="P21" s="84"/>
-      <c r="Q21" s="87"/>
+      <c r="P21" s="87"/>
+      <c r="Q21" s="90"/>
     </row>
   </sheetData>
   <mergeCells count="45">
@@ -3638,7 +3680,7 @@
     <mergeCell ref="A8:A12"/>
     <mergeCell ref="A13:A14"/>
   </mergeCells>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
fix bug validation CMND/CCCD of customer funtion update renting rooms
</commit_message>
<xml_diff>
--- a/SEP-VanLangHotel/Upload/Demo.xlsx
+++ b/SEP-VanLangHotel/Upload/Demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dangt\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7EAD0EB-8BF9-4BD9-BA6E-A7292FB104F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C594157D-1AF5-4CF7-801B-F8B4B585D078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="595" activeTab="1" xr2:uid="{E93DE5FD-DC7B-498D-86AD-F192523F8D5C}"/>
   </bookViews>
@@ -1829,6 +1829,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1868,23 +1883,23 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1895,6 +1910,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1904,37 +1937,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1943,70 +1964,49 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2341,40 +2341,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="83" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="80" t="s">
+      <c r="B1" s="85" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="80" t="s">
+      <c r="C1" s="85" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="80" t="s">
+      <c r="D1" s="85" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="80" t="s">
+      <c r="E1" s="85" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="82" t="s">
+      <c r="F1" s="87" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="74" t="s">
+      <c r="G1" s="79" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="76" t="s">
+      <c r="H1" s="81" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="79"/>
-      <c r="B2" s="81"/>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="77"/>
+      <c r="A2" s="84"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="82"/>
     </row>
     <row r="3" spans="1:8" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="48" t="s">
@@ -2398,7 +2398,7 @@
       <c r="G3" s="56" t="s">
         <v>118</v>
       </c>
-      <c r="H3" s="71" t="s">
+      <c r="H3" s="76" t="s">
         <v>87</v>
       </c>
     </row>
@@ -2424,7 +2424,7 @@
       <c r="G4" s="60" t="s">
         <v>120</v>
       </c>
-      <c r="H4" s="72"/>
+      <c r="H4" s="77"/>
     </row>
     <row r="5" spans="1:8" ht="22.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="48" t="s">
@@ -2448,7 +2448,7 @@
       <c r="G5" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="H5" s="72"/>
+      <c r="H5" s="77"/>
     </row>
     <row r="6" spans="1:8" ht="22.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="48" t="s">
@@ -2472,7 +2472,7 @@
       <c r="G6" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="72"/>
+      <c r="H6" s="77"/>
     </row>
     <row r="7" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="49" t="s">
@@ -2496,7 +2496,7 @@
       <c r="G7" s="57" t="s">
         <v>118</v>
       </c>
-      <c r="H7" s="72"/>
+      <c r="H7" s="77"/>
     </row>
     <row r="8" spans="1:8" ht="31.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="50" t="s">
@@ -2520,7 +2520,7 @@
       <c r="G8" s="61" t="s">
         <v>120</v>
       </c>
-      <c r="H8" s="72"/>
+      <c r="H8" s="77"/>
     </row>
     <row r="9" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="50" t="s">
@@ -2544,7 +2544,7 @@
       <c r="G9" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="72"/>
+      <c r="H9" s="77"/>
     </row>
     <row r="10" spans="1:8" ht="22.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="51" t="s">
@@ -2568,7 +2568,7 @@
       <c r="G10" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="H10" s="73"/>
+      <c r="H10" s="78"/>
     </row>
     <row r="11" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="48" t="s">
@@ -2978,8 +2978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1EC22DE-93F5-4706-915E-304A5F11A983}">
   <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="J3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3005,29 +3005,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="92" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="119"/>
-      <c r="C1" s="119"/>
-      <c r="D1" s="119"/>
-      <c r="E1" s="119"/>
-      <c r="F1" s="119"/>
-      <c r="G1" s="119"/>
-      <c r="H1" s="119"/>
-      <c r="I1" s="119"/>
-      <c r="J1" s="120"/>
-      <c r="K1" s="109" t="s">
+      <c r="B1" s="93"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="93"/>
+      <c r="H1" s="93"/>
+      <c r="I1" s="93"/>
+      <c r="J1" s="94"/>
+      <c r="K1" s="107" t="s">
         <v>35</v>
       </c>
-      <c r="L1" s="110"/>
-      <c r="M1" s="110"/>
-      <c r="N1" s="110"/>
-      <c r="O1" s="111"/>
-      <c r="P1" s="107" t="s">
+      <c r="L1" s="108"/>
+      <c r="M1" s="108"/>
+      <c r="N1" s="108"/>
+      <c r="O1" s="109"/>
+      <c r="P1" s="114" t="s">
         <v>85</v>
       </c>
-      <c r="Q1" s="108"/>
+      <c r="Q1" s="115"/>
     </row>
     <row r="2" spans="1:17" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="42" t="s">
@@ -3083,7 +3083,7 @@
       </c>
     </row>
     <row r="3" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="90">
+      <c r="A3" s="95">
         <v>1</v>
       </c>
       <c r="B3" s="16">
@@ -3096,7 +3096,7 @@
       <c r="E3" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="102" t="s">
+      <c r="F3" s="89" t="s">
         <v>5</v>
       </c>
       <c r="G3" s="11">
@@ -3108,33 +3108,33 @@
       <c r="I3" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="J3" s="93">
+      <c r="J3" s="104">
         <v>2</v>
       </c>
-      <c r="K3" s="96">
-        <v>1</v>
-      </c>
-      <c r="L3" s="99">
-        <v>1</v>
-      </c>
-      <c r="M3" s="99">
-        <v>1</v>
-      </c>
-      <c r="N3" s="99">
+      <c r="K3" s="123">
+        <v>1</v>
+      </c>
+      <c r="L3" s="127">
+        <v>1</v>
+      </c>
+      <c r="M3" s="127">
+        <v>1</v>
+      </c>
+      <c r="N3" s="127">
         <v>0</v>
       </c>
-      <c r="O3" s="93">
-        <v>1</v>
-      </c>
-      <c r="P3" s="87">
-        <v>44765</v>
-      </c>
-      <c r="Q3" s="84">
-        <v>44765</v>
+      <c r="O3" s="104">
+        <v>1</v>
+      </c>
+      <c r="P3" s="120">
+        <v>44768</v>
+      </c>
+      <c r="Q3" s="117">
+        <v>44768</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="91"/>
+      <c r="A4" s="96"/>
       <c r="B4" s="17">
         <v>2</v>
       </c>
@@ -3145,7 +3145,7 @@
         <v>39</v>
       </c>
       <c r="E4" s="7"/>
-      <c r="F4" s="103"/>
+      <c r="F4" s="90"/>
       <c r="G4" s="8">
         <v>39571</v>
       </c>
@@ -3155,17 +3155,17 @@
       <c r="I4" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="J4" s="94"/>
-      <c r="K4" s="97"/>
-      <c r="L4" s="100"/>
-      <c r="M4" s="100"/>
-      <c r="N4" s="100"/>
-      <c r="O4" s="94"/>
-      <c r="P4" s="88"/>
-      <c r="Q4" s="85"/>
+      <c r="J4" s="105"/>
+      <c r="K4" s="124"/>
+      <c r="L4" s="128"/>
+      <c r="M4" s="128"/>
+      <c r="N4" s="128"/>
+      <c r="O4" s="105"/>
+      <c r="P4" s="121"/>
+      <c r="Q4" s="118"/>
     </row>
     <row r="5" spans="1:17" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="91"/>
+      <c r="A5" s="96"/>
       <c r="B5" s="17">
         <v>3</v>
       </c>
@@ -3176,7 +3176,7 @@
         <v>37</v>
       </c>
       <c r="E5" s="7"/>
-      <c r="F5" s="103"/>
+      <c r="F5" s="90"/>
       <c r="G5" s="8">
         <v>39459</v>
       </c>
@@ -3186,17 +3186,17 @@
       <c r="I5" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="J5" s="94"/>
-      <c r="K5" s="97"/>
-      <c r="L5" s="100"/>
-      <c r="M5" s="100"/>
-      <c r="N5" s="100"/>
-      <c r="O5" s="94"/>
-      <c r="P5" s="88"/>
-      <c r="Q5" s="85"/>
+      <c r="J5" s="105"/>
+      <c r="K5" s="124"/>
+      <c r="L5" s="128"/>
+      <c r="M5" s="128"/>
+      <c r="N5" s="128"/>
+      <c r="O5" s="105"/>
+      <c r="P5" s="121"/>
+      <c r="Q5" s="118"/>
     </row>
     <row r="6" spans="1:17" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="91"/>
+      <c r="A6" s="96"/>
       <c r="B6" s="17">
         <v>4</v>
       </c>
@@ -3207,7 +3207,7 @@
         <v>39</v>
       </c>
       <c r="E6" s="7"/>
-      <c r="F6" s="103"/>
+      <c r="F6" s="90"/>
       <c r="G6" s="8">
         <v>40505</v>
       </c>
@@ -3217,17 +3217,17 @@
       <c r="I6" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="J6" s="94"/>
-      <c r="K6" s="97"/>
-      <c r="L6" s="100"/>
-      <c r="M6" s="100"/>
-      <c r="N6" s="100"/>
-      <c r="O6" s="94"/>
-      <c r="P6" s="88"/>
-      <c r="Q6" s="85"/>
+      <c r="J6" s="105"/>
+      <c r="K6" s="124"/>
+      <c r="L6" s="128"/>
+      <c r="M6" s="128"/>
+      <c r="N6" s="128"/>
+      <c r="O6" s="105"/>
+      <c r="P6" s="121"/>
+      <c r="Q6" s="118"/>
     </row>
     <row r="7" spans="1:17" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="92"/>
+      <c r="A7" s="97"/>
       <c r="B7" s="18">
         <v>5</v>
       </c>
@@ -3238,7 +3238,7 @@
         <v>40</v>
       </c>
       <c r="E7" s="13"/>
-      <c r="F7" s="104"/>
+      <c r="F7" s="91"/>
       <c r="G7" s="14">
         <v>41149</v>
       </c>
@@ -3248,17 +3248,17 @@
       <c r="I7" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="J7" s="95"/>
-      <c r="K7" s="98"/>
-      <c r="L7" s="101"/>
-      <c r="M7" s="101"/>
-      <c r="N7" s="101"/>
-      <c r="O7" s="95"/>
-      <c r="P7" s="88"/>
-      <c r="Q7" s="85"/>
+      <c r="J7" s="106"/>
+      <c r="K7" s="126"/>
+      <c r="L7" s="130"/>
+      <c r="M7" s="130"/>
+      <c r="N7" s="130"/>
+      <c r="O7" s="106"/>
+      <c r="P7" s="121"/>
+      <c r="Q7" s="118"/>
     </row>
     <row r="8" spans="1:17" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A8" s="90">
+      <c r="A8" s="95">
         <v>2</v>
       </c>
       <c r="B8" s="16">
@@ -3271,7 +3271,7 @@
       <c r="E8" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="F8" s="102" t="s">
+      <c r="F8" s="89" t="s">
         <v>90</v>
       </c>
       <c r="G8" s="11">
@@ -3283,29 +3283,29 @@
       <c r="I8" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="J8" s="93">
+      <c r="J8" s="104">
         <v>2</v>
       </c>
-      <c r="K8" s="96">
-        <v>1</v>
-      </c>
-      <c r="L8" s="99">
+      <c r="K8" s="123">
+        <v>1</v>
+      </c>
+      <c r="L8" s="127">
         <v>0</v>
       </c>
-      <c r="M8" s="99">
-        <v>1</v>
-      </c>
-      <c r="N8" s="99">
+      <c r="M8" s="127">
+        <v>1</v>
+      </c>
+      <c r="N8" s="127">
         <v>0</v>
       </c>
-      <c r="O8" s="93">
+      <c r="O8" s="104">
         <v>0</v>
       </c>
-      <c r="P8" s="88"/>
-      <c r="Q8" s="85"/>
+      <c r="P8" s="121"/>
+      <c r="Q8" s="118"/>
     </row>
     <row r="9" spans="1:17" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A9" s="91"/>
+      <c r="A9" s="96"/>
       <c r="B9" s="17">
         <v>2</v>
       </c>
@@ -3316,7 +3316,7 @@
         <v>44</v>
       </c>
       <c r="E9" s="7"/>
-      <c r="F9" s="103"/>
+      <c r="F9" s="90"/>
       <c r="G9" s="8">
         <v>39826</v>
       </c>
@@ -3326,17 +3326,17 @@
       <c r="I9" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="J9" s="94"/>
-      <c r="K9" s="97"/>
-      <c r="L9" s="100"/>
-      <c r="M9" s="100"/>
-      <c r="N9" s="100"/>
-      <c r="O9" s="94"/>
-      <c r="P9" s="88"/>
-      <c r="Q9" s="85"/>
+      <c r="J9" s="105"/>
+      <c r="K9" s="124"/>
+      <c r="L9" s="128"/>
+      <c r="M9" s="128"/>
+      <c r="N9" s="128"/>
+      <c r="O9" s="105"/>
+      <c r="P9" s="121"/>
+      <c r="Q9" s="118"/>
     </row>
     <row r="10" spans="1:17" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A10" s="91"/>
+      <c r="A10" s="96"/>
       <c r="B10" s="17">
         <v>3</v>
       </c>
@@ -3347,7 +3347,7 @@
         <v>44</v>
       </c>
       <c r="E10" s="7"/>
-      <c r="F10" s="103"/>
+      <c r="F10" s="90"/>
       <c r="G10" s="8">
         <v>40291</v>
       </c>
@@ -3357,17 +3357,17 @@
       <c r="I10" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="J10" s="94"/>
-      <c r="K10" s="97"/>
-      <c r="L10" s="100"/>
-      <c r="M10" s="100"/>
-      <c r="N10" s="100"/>
-      <c r="O10" s="94"/>
-      <c r="P10" s="88"/>
-      <c r="Q10" s="85"/>
+      <c r="J10" s="105"/>
+      <c r="K10" s="124"/>
+      <c r="L10" s="128"/>
+      <c r="M10" s="128"/>
+      <c r="N10" s="128"/>
+      <c r="O10" s="105"/>
+      <c r="P10" s="121"/>
+      <c r="Q10" s="118"/>
     </row>
     <row r="11" spans="1:17" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A11" s="91"/>
+      <c r="A11" s="96"/>
       <c r="B11" s="17">
         <v>4</v>
       </c>
@@ -3378,7 +3378,7 @@
         <v>44</v>
       </c>
       <c r="E11" s="7"/>
-      <c r="F11" s="103"/>
+      <c r="F11" s="90"/>
       <c r="G11" s="8">
         <v>40497</v>
       </c>
@@ -3388,48 +3388,48 @@
       <c r="I11" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="J11" s="94"/>
-      <c r="K11" s="97"/>
-      <c r="L11" s="100"/>
-      <c r="M11" s="100"/>
-      <c r="N11" s="100"/>
-      <c r="O11" s="94"/>
-      <c r="P11" s="88"/>
-      <c r="Q11" s="85"/>
+      <c r="J11" s="105"/>
+      <c r="K11" s="124"/>
+      <c r="L11" s="128"/>
+      <c r="M11" s="128"/>
+      <c r="N11" s="128"/>
+      <c r="O11" s="105"/>
+      <c r="P11" s="121"/>
+      <c r="Q11" s="118"/>
     </row>
     <row r="12" spans="1:17" ht="26.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="122"/>
-      <c r="B12" s="123">
+      <c r="A12" s="113"/>
+      <c r="B12" s="71">
         <v>5</v>
       </c>
-      <c r="C12" s="124" t="s">
+      <c r="C12" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="123" t="s">
+      <c r="D12" s="71" t="s">
         <v>44</v>
       </c>
-      <c r="E12" s="125"/>
-      <c r="F12" s="103"/>
-      <c r="G12" s="126">
+      <c r="E12" s="73"/>
+      <c r="F12" s="90"/>
+      <c r="G12" s="74">
         <v>39894</v>
       </c>
-      <c r="H12" s="123">
-        <v>1</v>
-      </c>
-      <c r="I12" s="127" t="s">
+      <c r="H12" s="71">
+        <v>1</v>
+      </c>
+      <c r="I12" s="75" t="s">
         <v>124</v>
       </c>
-      <c r="J12" s="128"/>
-      <c r="K12" s="129"/>
-      <c r="L12" s="130"/>
-      <c r="M12" s="130"/>
-      <c r="N12" s="130"/>
-      <c r="O12" s="128"/>
-      <c r="P12" s="88"/>
-      <c r="Q12" s="85"/>
+      <c r="J12" s="116"/>
+      <c r="K12" s="125"/>
+      <c r="L12" s="129"/>
+      <c r="M12" s="129"/>
+      <c r="N12" s="129"/>
+      <c r="O12" s="116"/>
+      <c r="P12" s="121"/>
+      <c r="Q12" s="118"/>
     </row>
     <row r="13" spans="1:17" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="92"/>
+      <c r="A13" s="97"/>
       <c r="B13" s="18">
         <v>6</v>
       </c>
@@ -3440,7 +3440,7 @@
         <v>44</v>
       </c>
       <c r="E13" s="13"/>
-      <c r="F13" s="104"/>
+      <c r="F13" s="91"/>
       <c r="G13" s="14">
         <v>40231</v>
       </c>
@@ -3450,17 +3450,17 @@
       <c r="I13" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="J13" s="95"/>
-      <c r="K13" s="98"/>
-      <c r="L13" s="101"/>
-      <c r="M13" s="101"/>
-      <c r="N13" s="101"/>
-      <c r="O13" s="95"/>
-      <c r="P13" s="88"/>
-      <c r="Q13" s="85"/>
+      <c r="J13" s="106"/>
+      <c r="K13" s="126"/>
+      <c r="L13" s="130"/>
+      <c r="M13" s="130"/>
+      <c r="N13" s="130"/>
+      <c r="O13" s="106"/>
+      <c r="P13" s="121"/>
+      <c r="Q13" s="118"/>
     </row>
     <row r="14" spans="1:17" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A14" s="90">
+      <c r="A14" s="95">
         <v>3</v>
       </c>
       <c r="B14" s="16">
@@ -3473,7 +3473,7 @@
       <c r="E14" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="102" t="s">
+      <c r="F14" s="89" t="s">
         <v>51</v>
       </c>
       <c r="G14" s="11">
@@ -3485,29 +3485,29 @@
       <c r="I14" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="J14" s="93">
-        <v>1</v>
-      </c>
-      <c r="K14" s="105">
+      <c r="J14" s="104">
+        <v>1</v>
+      </c>
+      <c r="K14" s="110">
         <v>0</v>
       </c>
-      <c r="L14" s="112">
+      <c r="L14" s="98">
         <v>0</v>
       </c>
-      <c r="M14" s="112">
-        <v>1</v>
-      </c>
-      <c r="N14" s="112">
+      <c r="M14" s="98">
+        <v>1</v>
+      </c>
+      <c r="N14" s="98">
         <v>0</v>
       </c>
-      <c r="O14" s="114">
-        <v>1</v>
-      </c>
-      <c r="P14" s="88"/>
-      <c r="Q14" s="85"/>
+      <c r="O14" s="101">
+        <v>1</v>
+      </c>
+      <c r="P14" s="121"/>
+      <c r="Q14" s="118"/>
     </row>
     <row r="15" spans="1:17" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="92"/>
+      <c r="A15" s="97"/>
       <c r="B15" s="18">
         <v>2</v>
       </c>
@@ -3520,7 +3520,7 @@
       <c r="E15" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="F15" s="104"/>
+      <c r="F15" s="91"/>
       <c r="G15" s="14">
         <v>37459</v>
       </c>
@@ -3530,17 +3530,17 @@
       <c r="I15" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="J15" s="95"/>
-      <c r="K15" s="106"/>
-      <c r="L15" s="113"/>
-      <c r="M15" s="113"/>
-      <c r="N15" s="113"/>
-      <c r="O15" s="115"/>
-      <c r="P15" s="88"/>
-      <c r="Q15" s="85"/>
+      <c r="J15" s="106"/>
+      <c r="K15" s="112"/>
+      <c r="L15" s="100"/>
+      <c r="M15" s="100"/>
+      <c r="N15" s="100"/>
+      <c r="O15" s="103"/>
+      <c r="P15" s="121"/>
+      <c r="Q15" s="118"/>
     </row>
     <row r="16" spans="1:17" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A16" s="90">
+      <c r="A16" s="95">
         <v>4</v>
       </c>
       <c r="B16" s="16">
@@ -3553,7 +3553,7 @@
       <c r="E16" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="F16" s="102" t="s">
+      <c r="F16" s="89" t="s">
         <v>49</v>
       </c>
       <c r="G16" s="11">
@@ -3565,29 +3565,29 @@
       <c r="I16" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="J16" s="93">
+      <c r="J16" s="104">
         <v>2</v>
       </c>
-      <c r="K16" s="105">
+      <c r="K16" s="110">
         <v>0</v>
       </c>
-      <c r="L16" s="112">
-        <v>1</v>
-      </c>
-      <c r="M16" s="112">
+      <c r="L16" s="98">
+        <v>1</v>
+      </c>
+      <c r="M16" s="98">
         <v>0</v>
       </c>
-      <c r="N16" s="112">
+      <c r="N16" s="98">
         <v>0</v>
       </c>
-      <c r="O16" s="114">
-        <v>1</v>
-      </c>
-      <c r="P16" s="88"/>
-      <c r="Q16" s="85"/>
+      <c r="O16" s="101">
+        <v>1</v>
+      </c>
+      <c r="P16" s="121"/>
+      <c r="Q16" s="118"/>
     </row>
     <row r="17" spans="1:17" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A17" s="91"/>
+      <c r="A17" s="96"/>
       <c r="B17" s="17">
         <v>2</v>
       </c>
@@ -3600,7 +3600,7 @@
       <c r="E17" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="F17" s="103"/>
+      <c r="F17" s="90"/>
       <c r="G17" s="8">
         <v>38555</v>
       </c>
@@ -3610,17 +3610,17 @@
       <c r="I17" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="J17" s="94"/>
-      <c r="K17" s="116"/>
-      <c r="L17" s="117"/>
-      <c r="M17" s="117"/>
-      <c r="N17" s="117"/>
-      <c r="O17" s="121"/>
-      <c r="P17" s="88"/>
-      <c r="Q17" s="85"/>
+      <c r="J17" s="105"/>
+      <c r="K17" s="111"/>
+      <c r="L17" s="99"/>
+      <c r="M17" s="99"/>
+      <c r="N17" s="99"/>
+      <c r="O17" s="102"/>
+      <c r="P17" s="121"/>
+      <c r="Q17" s="118"/>
     </row>
     <row r="18" spans="1:17" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A18" s="91"/>
+      <c r="A18" s="96"/>
       <c r="B18" s="17">
         <v>3</v>
       </c>
@@ -3633,7 +3633,7 @@
       <c r="E18" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="F18" s="103"/>
+      <c r="F18" s="90"/>
       <c r="G18" s="8">
         <v>37667</v>
       </c>
@@ -3643,17 +3643,17 @@
       <c r="I18" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="J18" s="94"/>
-      <c r="K18" s="116"/>
-      <c r="L18" s="117"/>
-      <c r="M18" s="117"/>
-      <c r="N18" s="117"/>
-      <c r="O18" s="121"/>
-      <c r="P18" s="88"/>
-      <c r="Q18" s="85"/>
+      <c r="J18" s="105"/>
+      <c r="K18" s="111"/>
+      <c r="L18" s="99"/>
+      <c r="M18" s="99"/>
+      <c r="N18" s="99"/>
+      <c r="O18" s="102"/>
+      <c r="P18" s="121"/>
+      <c r="Q18" s="118"/>
     </row>
     <row r="19" spans="1:17" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="92"/>
+      <c r="A19" s="97"/>
       <c r="B19" s="18">
         <v>4</v>
       </c>
@@ -3666,7 +3666,7 @@
       <c r="E19" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="F19" s="104"/>
+      <c r="F19" s="91"/>
       <c r="G19" s="14">
         <v>37485</v>
       </c>
@@ -3676,17 +3676,17 @@
       <c r="I19" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="J19" s="95"/>
-      <c r="K19" s="106"/>
-      <c r="L19" s="113"/>
-      <c r="M19" s="113"/>
-      <c r="N19" s="113"/>
-      <c r="O19" s="115"/>
-      <c r="P19" s="88"/>
-      <c r="Q19" s="85"/>
+      <c r="J19" s="106"/>
+      <c r="K19" s="112"/>
+      <c r="L19" s="100"/>
+      <c r="M19" s="100"/>
+      <c r="N19" s="100"/>
+      <c r="O19" s="103"/>
+      <c r="P19" s="121"/>
+      <c r="Q19" s="118"/>
     </row>
     <row r="20" spans="1:17" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A20" s="90">
+      <c r="A20" s="95">
         <v>5</v>
       </c>
       <c r="B20" s="16">
@@ -3699,7 +3699,7 @@
       <c r="E20" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="F20" s="102" t="s">
+      <c r="F20" s="89" t="s">
         <v>52</v>
       </c>
       <c r="G20" s="11">
@@ -3711,29 +3711,29 @@
       <c r="I20" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="J20" s="93">
+      <c r="J20" s="104">
         <v>2</v>
       </c>
-      <c r="K20" s="105">
-        <v>1</v>
-      </c>
-      <c r="L20" s="112">
+      <c r="K20" s="110">
+        <v>1</v>
+      </c>
+      <c r="L20" s="98">
         <v>0</v>
       </c>
-      <c r="M20" s="112">
-        <v>1</v>
-      </c>
-      <c r="N20" s="112">
-        <v>1</v>
-      </c>
-      <c r="O20" s="114">
-        <v>1</v>
-      </c>
-      <c r="P20" s="88"/>
-      <c r="Q20" s="85"/>
+      <c r="M20" s="98">
+        <v>1</v>
+      </c>
+      <c r="N20" s="98">
+        <v>1</v>
+      </c>
+      <c r="O20" s="101">
+        <v>1</v>
+      </c>
+      <c r="P20" s="121"/>
+      <c r="Q20" s="118"/>
     </row>
     <row r="21" spans="1:17" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A21" s="91"/>
+      <c r="A21" s="96"/>
       <c r="B21" s="17">
         <v>2</v>
       </c>
@@ -3744,7 +3744,7 @@
         <v>69</v>
       </c>
       <c r="E21" s="7"/>
-      <c r="F21" s="103"/>
+      <c r="F21" s="90"/>
       <c r="G21" s="8">
         <v>40016</v>
       </c>
@@ -3754,17 +3754,17 @@
       <c r="I21" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="J21" s="94"/>
-      <c r="K21" s="116"/>
-      <c r="L21" s="117"/>
-      <c r="M21" s="117"/>
-      <c r="N21" s="117"/>
-      <c r="O21" s="121"/>
-      <c r="P21" s="88"/>
-      <c r="Q21" s="85"/>
+      <c r="J21" s="105"/>
+      <c r="K21" s="111"/>
+      <c r="L21" s="99"/>
+      <c r="M21" s="99"/>
+      <c r="N21" s="99"/>
+      <c r="O21" s="102"/>
+      <c r="P21" s="121"/>
+      <c r="Q21" s="118"/>
     </row>
     <row r="22" spans="1:17" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="92"/>
+      <c r="A22" s="97"/>
       <c r="B22" s="18">
         <v>3</v>
       </c>
@@ -3775,7 +3775,7 @@
         <v>70</v>
       </c>
       <c r="E22" s="13"/>
-      <c r="F22" s="104"/>
+      <c r="F22" s="91"/>
       <c r="G22" s="14">
         <v>40224</v>
       </c>
@@ -3785,14 +3785,14 @@
       <c r="I22" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="J22" s="95"/>
-      <c r="K22" s="106"/>
-      <c r="L22" s="113"/>
-      <c r="M22" s="113"/>
-      <c r="N22" s="113"/>
-      <c r="O22" s="115"/>
-      <c r="P22" s="88"/>
-      <c r="Q22" s="85"/>
+      <c r="J22" s="106"/>
+      <c r="K22" s="112"/>
+      <c r="L22" s="100"/>
+      <c r="M22" s="100"/>
+      <c r="N22" s="100"/>
+      <c r="O22" s="103"/>
+      <c r="P22" s="121"/>
+      <c r="Q22" s="118"/>
     </row>
     <row r="23" spans="1:17" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="63">
@@ -3838,17 +3838,34 @@
       <c r="O23" s="69">
         <v>1</v>
       </c>
-      <c r="P23" s="89"/>
-      <c r="Q23" s="86"/>
+      <c r="P23" s="122"/>
+      <c r="Q23" s="119"/>
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="F16:F19"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="N16:N19"/>
-    <mergeCell ref="O16:O19"/>
-    <mergeCell ref="J16:J19"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="O3:O7"/>
+    <mergeCell ref="K8:K13"/>
+    <mergeCell ref="L8:L13"/>
+    <mergeCell ref="M8:M13"/>
+    <mergeCell ref="N8:N13"/>
+    <mergeCell ref="O8:O13"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="K3:K7"/>
+    <mergeCell ref="L3:L7"/>
+    <mergeCell ref="M3:M7"/>
+    <mergeCell ref="N3:N7"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="J3:J7"/>
+    <mergeCell ref="J8:J13"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="F3:F7"/>
+    <mergeCell ref="F8:F13"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="Q3:Q23"/>
+    <mergeCell ref="P3:P23"/>
     <mergeCell ref="J20:J22"/>
     <mergeCell ref="K1:O1"/>
     <mergeCell ref="L14:L15"/>
@@ -3863,31 +3880,14 @@
     <mergeCell ref="M20:M22"/>
     <mergeCell ref="N20:N22"/>
     <mergeCell ref="O20:O22"/>
+    <mergeCell ref="F16:F19"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="N16:N19"/>
+    <mergeCell ref="O16:O19"/>
+    <mergeCell ref="J16:J19"/>
     <mergeCell ref="A8:A13"/>
     <mergeCell ref="A14:A15"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="J3:J7"/>
-    <mergeCell ref="J8:J13"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="F3:F7"/>
-    <mergeCell ref="F8:F13"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="Q3:Q23"/>
-    <mergeCell ref="P3:P23"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="O3:O7"/>
-    <mergeCell ref="K8:K13"/>
-    <mergeCell ref="L8:L13"/>
-    <mergeCell ref="M8:M13"/>
-    <mergeCell ref="N8:N13"/>
-    <mergeCell ref="O8:O13"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="K3:K7"/>
-    <mergeCell ref="L3:L7"/>
-    <mergeCell ref="M3:M7"/>
-    <mergeCell ref="N3:N7"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3896,9 +3896,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4111,27 +4114,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D6B5C1E-8E64-4C3F-8B9C-ADE9CAA17D4A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8E843C9-AFC0-407A-892D-C6431DD2F37F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="23dced98-c23c-4266-be03-749ab8bb2b21"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="45e2578b-5781-47e1-85a2-a2bca000d7fe"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4156,9 +4147,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8E843C9-AFC0-407A-892D-C6431DD2F37F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D6B5C1E-8E64-4C3F-8B9C-ADE9CAA17D4A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="23dced98-c23c-4266-be03-749ab8bb2b21"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="45e2578b-5781-47e1-85a2-a2bca000d7fe"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add function management tour view Nhân viên
</commit_message>
<xml_diff>
--- a/SEP-VanLangHotel/Upload/Demo.xlsx
+++ b/SEP-VanLangHotel/Upload/Demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dangt\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E0A3767-212A-4646-BED1-ED309F4CA83F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D420539C-7E4D-4275-84E9-04DB1AB632F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="595" activeTab="1" xr2:uid="{E93DE5FD-DC7B-498D-86AD-F192523F8D5C}"/>
+    <workbookView xWindow="2472" yWindow="2472" windowWidth="17280" windowHeight="8880" tabRatio="595" activeTab="1" xr2:uid="{E93DE5FD-DC7B-498D-86AD-F192523F8D5C}"/>
   </bookViews>
   <sheets>
     <sheet name="Bảng giá &amp; Quy tắc" sheetId="4" r:id="rId1"/>
@@ -1943,6 +1943,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1976,12 +1985,6 @@
     <xf numFmtId="0" fontId="12" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1989,9 +1992,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2978,8 +2978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1EC22DE-93F5-4706-915E-304A5F11A983}">
   <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+    <sheetView tabSelected="1" topLeftCell="N3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3017,17 +3017,17 @@
       <c r="H1" s="128"/>
       <c r="I1" s="128"/>
       <c r="J1" s="129"/>
-      <c r="K1" s="117" t="s">
+      <c r="K1" s="120" t="s">
         <v>35</v>
       </c>
-      <c r="L1" s="118"/>
-      <c r="M1" s="118"/>
-      <c r="N1" s="118"/>
-      <c r="O1" s="119"/>
-      <c r="P1" s="109" t="s">
+      <c r="L1" s="121"/>
+      <c r="M1" s="121"/>
+      <c r="N1" s="121"/>
+      <c r="O1" s="122"/>
+      <c r="P1" s="112" t="s">
         <v>85</v>
       </c>
-      <c r="Q1" s="110"/>
+      <c r="Q1" s="113"/>
     </row>
     <row r="2" spans="1:17" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="42" t="s">
@@ -3126,11 +3126,11 @@
       <c r="O3" s="92">
         <v>1</v>
       </c>
-      <c r="P3" s="114">
-        <v>44770</v>
-      </c>
-      <c r="Q3" s="111">
-        <v>44770</v>
+      <c r="P3" s="117">
+        <v>44783</v>
+      </c>
+      <c r="Q3" s="114">
+        <v>44783</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
@@ -3161,8 +3161,8 @@
       <c r="M4" s="100"/>
       <c r="N4" s="100"/>
       <c r="O4" s="93"/>
-      <c r="P4" s="115"/>
-      <c r="Q4" s="112"/>
+      <c r="P4" s="118"/>
+      <c r="Q4" s="115"/>
     </row>
     <row r="5" spans="1:17" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="90"/>
@@ -3192,8 +3192,8 @@
       <c r="M5" s="100"/>
       <c r="N5" s="100"/>
       <c r="O5" s="93"/>
-      <c r="P5" s="115"/>
-      <c r="Q5" s="112"/>
+      <c r="P5" s="118"/>
+      <c r="Q5" s="115"/>
     </row>
     <row r="6" spans="1:17" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="90"/>
@@ -3223,8 +3223,8 @@
       <c r="M6" s="100"/>
       <c r="N6" s="100"/>
       <c r="O6" s="93"/>
-      <c r="P6" s="115"/>
-      <c r="Q6" s="112"/>
+      <c r="P6" s="118"/>
+      <c r="Q6" s="115"/>
     </row>
     <row r="7" spans="1:17" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="91"/>
@@ -3254,8 +3254,8 @@
       <c r="M7" s="102"/>
       <c r="N7" s="102"/>
       <c r="O7" s="94"/>
-      <c r="P7" s="115"/>
-      <c r="Q7" s="112"/>
+      <c r="P7" s="118"/>
+      <c r="Q7" s="115"/>
     </row>
     <row r="8" spans="1:17" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A8" s="89">
@@ -3301,8 +3301,8 @@
       <c r="O8" s="92">
         <v>0</v>
       </c>
-      <c r="P8" s="115"/>
-      <c r="Q8" s="112"/>
+      <c r="P8" s="118"/>
+      <c r="Q8" s="115"/>
     </row>
     <row r="9" spans="1:17" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A9" s="90"/>
@@ -3332,8 +3332,8 @@
       <c r="M9" s="100"/>
       <c r="N9" s="100"/>
       <c r="O9" s="93"/>
-      <c r="P9" s="115"/>
-      <c r="Q9" s="112"/>
+      <c r="P9" s="118"/>
+      <c r="Q9" s="115"/>
     </row>
     <row r="10" spans="1:17" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A10" s="90"/>
@@ -3363,8 +3363,8 @@
       <c r="M10" s="100"/>
       <c r="N10" s="100"/>
       <c r="O10" s="93"/>
-      <c r="P10" s="115"/>
-      <c r="Q10" s="112"/>
+      <c r="P10" s="118"/>
+      <c r="Q10" s="115"/>
     </row>
     <row r="11" spans="1:17" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A11" s="90"/>
@@ -3394,8 +3394,8 @@
       <c r="M11" s="100"/>
       <c r="N11" s="100"/>
       <c r="O11" s="93"/>
-      <c r="P11" s="115"/>
-      <c r="Q11" s="112"/>
+      <c r="P11" s="118"/>
+      <c r="Q11" s="115"/>
     </row>
     <row r="12" spans="1:17" ht="26.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="130"/>
@@ -3425,8 +3425,8 @@
       <c r="M12" s="101"/>
       <c r="N12" s="101"/>
       <c r="O12" s="103"/>
-      <c r="P12" s="115"/>
-      <c r="Q12" s="112"/>
+      <c r="P12" s="118"/>
+      <c r="Q12" s="115"/>
     </row>
     <row r="13" spans="1:17" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="91"/>
@@ -3456,8 +3456,8 @@
       <c r="M13" s="102"/>
       <c r="N13" s="102"/>
       <c r="O13" s="94"/>
-      <c r="P13" s="115"/>
-      <c r="Q13" s="112"/>
+      <c r="P13" s="118"/>
+      <c r="Q13" s="115"/>
     </row>
     <row r="14" spans="1:17" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A14" s="89">
@@ -3491,20 +3491,20 @@
       <c r="K14" s="107">
         <v>0</v>
       </c>
-      <c r="L14" s="120">
+      <c r="L14" s="109">
         <v>0</v>
       </c>
-      <c r="M14" s="120">
-        <v>1</v>
-      </c>
-      <c r="N14" s="120">
+      <c r="M14" s="109">
+        <v>1</v>
+      </c>
+      <c r="N14" s="109">
         <v>0</v>
       </c>
-      <c r="O14" s="122">
-        <v>1</v>
-      </c>
-      <c r="P14" s="115"/>
-      <c r="Q14" s="112"/>
+      <c r="O14" s="123">
+        <v>1</v>
+      </c>
+      <c r="P14" s="118"/>
+      <c r="Q14" s="115"/>
     </row>
     <row r="15" spans="1:17" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="91"/>
@@ -3532,12 +3532,12 @@
       </c>
       <c r="J15" s="94"/>
       <c r="K15" s="108"/>
-      <c r="L15" s="121"/>
-      <c r="M15" s="121"/>
-      <c r="N15" s="121"/>
-      <c r="O15" s="123"/>
-      <c r="P15" s="115"/>
-      <c r="Q15" s="112"/>
+      <c r="L15" s="111"/>
+      <c r="M15" s="111"/>
+      <c r="N15" s="111"/>
+      <c r="O15" s="124"/>
+      <c r="P15" s="118"/>
+      <c r="Q15" s="115"/>
     </row>
     <row r="16" spans="1:17" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A16" s="89">
@@ -3571,20 +3571,20 @@
       <c r="K16" s="107">
         <v>0</v>
       </c>
-      <c r="L16" s="120">
-        <v>1</v>
-      </c>
-      <c r="M16" s="120">
+      <c r="L16" s="109">
+        <v>1</v>
+      </c>
+      <c r="M16" s="109">
         <v>0</v>
       </c>
-      <c r="N16" s="120">
+      <c r="N16" s="109">
         <v>0</v>
       </c>
-      <c r="O16" s="122">
-        <v>1</v>
-      </c>
-      <c r="P16" s="115"/>
-      <c r="Q16" s="112"/>
+      <c r="O16" s="123">
+        <v>1</v>
+      </c>
+      <c r="P16" s="118"/>
+      <c r="Q16" s="115"/>
     </row>
     <row r="17" spans="1:17" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A17" s="90"/>
@@ -3611,13 +3611,13 @@
         <v>73</v>
       </c>
       <c r="J17" s="93"/>
-      <c r="K17" s="124"/>
-      <c r="L17" s="125"/>
-      <c r="M17" s="125"/>
-      <c r="N17" s="125"/>
+      <c r="K17" s="125"/>
+      <c r="L17" s="110"/>
+      <c r="M17" s="110"/>
+      <c r="N17" s="110"/>
       <c r="O17" s="126"/>
-      <c r="P17" s="115"/>
-      <c r="Q17" s="112"/>
+      <c r="P17" s="118"/>
+      <c r="Q17" s="115"/>
     </row>
     <row r="18" spans="1:17" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A18" s="90"/>
@@ -3644,13 +3644,13 @@
         <v>74</v>
       </c>
       <c r="J18" s="93"/>
-      <c r="K18" s="124"/>
-      <c r="L18" s="125"/>
-      <c r="M18" s="125"/>
-      <c r="N18" s="125"/>
+      <c r="K18" s="125"/>
+      <c r="L18" s="110"/>
+      <c r="M18" s="110"/>
+      <c r="N18" s="110"/>
       <c r="O18" s="126"/>
-      <c r="P18" s="115"/>
-      <c r="Q18" s="112"/>
+      <c r="P18" s="118"/>
+      <c r="Q18" s="115"/>
     </row>
     <row r="19" spans="1:17" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="91"/>
@@ -3678,12 +3678,12 @@
       </c>
       <c r="J19" s="94"/>
       <c r="K19" s="108"/>
-      <c r="L19" s="121"/>
-      <c r="M19" s="121"/>
-      <c r="N19" s="121"/>
-      <c r="O19" s="123"/>
-      <c r="P19" s="115"/>
-      <c r="Q19" s="112"/>
+      <c r="L19" s="111"/>
+      <c r="M19" s="111"/>
+      <c r="N19" s="111"/>
+      <c r="O19" s="124"/>
+      <c r="P19" s="118"/>
+      <c r="Q19" s="115"/>
     </row>
     <row r="20" spans="1:17" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A20" s="89">
@@ -3717,20 +3717,20 @@
       <c r="K20" s="107">
         <v>1</v>
       </c>
-      <c r="L20" s="120">
+      <c r="L20" s="109">
         <v>0</v>
       </c>
-      <c r="M20" s="120">
-        <v>1</v>
-      </c>
-      <c r="N20" s="120">
-        <v>1</v>
-      </c>
-      <c r="O20" s="122">
-        <v>1</v>
-      </c>
-      <c r="P20" s="115"/>
-      <c r="Q20" s="112"/>
+      <c r="M20" s="109">
+        <v>1</v>
+      </c>
+      <c r="N20" s="109">
+        <v>1</v>
+      </c>
+      <c r="O20" s="123">
+        <v>1</v>
+      </c>
+      <c r="P20" s="118"/>
+      <c r="Q20" s="115"/>
     </row>
     <row r="21" spans="1:17" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A21" s="90"/>
@@ -3755,13 +3755,13 @@
         <v>82</v>
       </c>
       <c r="J21" s="93"/>
-      <c r="K21" s="124"/>
-      <c r="L21" s="125"/>
-      <c r="M21" s="125"/>
-      <c r="N21" s="125"/>
+      <c r="K21" s="125"/>
+      <c r="L21" s="110"/>
+      <c r="M21" s="110"/>
+      <c r="N21" s="110"/>
       <c r="O21" s="126"/>
-      <c r="P21" s="115"/>
-      <c r="Q21" s="112"/>
+      <c r="P21" s="118"/>
+      <c r="Q21" s="115"/>
     </row>
     <row r="22" spans="1:17" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="91"/>
@@ -3787,12 +3787,12 @@
       </c>
       <c r="J22" s="94"/>
       <c r="K22" s="108"/>
-      <c r="L22" s="121"/>
-      <c r="M22" s="121"/>
-      <c r="N22" s="121"/>
-      <c r="O22" s="123"/>
-      <c r="P22" s="115"/>
-      <c r="Q22" s="112"/>
+      <c r="L22" s="111"/>
+      <c r="M22" s="111"/>
+      <c r="N22" s="111"/>
+      <c r="O22" s="124"/>
+      <c r="P22" s="118"/>
+      <c r="Q22" s="115"/>
     </row>
     <row r="23" spans="1:17" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="63">
@@ -3838,8 +3838,8 @@
       <c r="O23" s="69">
         <v>1</v>
       </c>
-      <c r="P23" s="116"/>
-      <c r="Q23" s="113"/>
+      <c r="P23" s="119"/>
+      <c r="Q23" s="116"/>
     </row>
   </sheetData>
   <mergeCells count="45">

</xml_diff>

<commit_message>
Add funtion statistic revenue management. Build version 3.0
</commit_message>
<xml_diff>
--- a/SEP-VanLangHotel/Upload/Demo.xlsx
+++ b/SEP-VanLangHotel/Upload/Demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dangt\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{474C5FB7-66AE-4FAA-89B4-1F8B1A20D3B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA9C1E8C-5D64-4EBF-AA89-3FB6B6F9CBFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="595" activeTab="1" xr2:uid="{E93DE5FD-DC7B-498D-86AD-F192523F8D5C}"/>
   </bookViews>
@@ -1883,6 +1883,51 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1890,6 +1935,66 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1901,112 +2006,7 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2979,7 +2979,7 @@
   <dimension ref="A1:Q23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="N3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="T14" sqref="T14"/>
+      <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3005,18 +3005,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="127" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="93"/>
-      <c r="C1" s="93"/>
-      <c r="D1" s="93"/>
-      <c r="E1" s="93"/>
-      <c r="F1" s="93"/>
-      <c r="G1" s="93"/>
-      <c r="H1" s="93"/>
-      <c r="I1" s="93"/>
-      <c r="J1" s="94"/>
+      <c r="B1" s="128"/>
+      <c r="C1" s="128"/>
+      <c r="D1" s="128"/>
+      <c r="E1" s="128"/>
+      <c r="F1" s="128"/>
+      <c r="G1" s="128"/>
+      <c r="H1" s="128"/>
+      <c r="I1" s="128"/>
+      <c r="J1" s="129"/>
       <c r="K1" s="120" t="s">
         <v>35</v>
       </c>
@@ -3024,10 +3024,10 @@
       <c r="M1" s="121"/>
       <c r="N1" s="121"/>
       <c r="O1" s="122"/>
-      <c r="P1" s="111" t="s">
+      <c r="P1" s="112" t="s">
         <v>85</v>
       </c>
-      <c r="Q1" s="112"/>
+      <c r="Q1" s="113"/>
     </row>
     <row r="2" spans="1:17" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="42" t="s">
@@ -3083,7 +3083,7 @@
       </c>
     </row>
     <row r="3" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="95">
+      <c r="A3" s="89">
         <v>1</v>
       </c>
       <c r="B3" s="16">
@@ -3096,7 +3096,7 @@
       <c r="E3" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="89" t="s">
+      <c r="F3" s="104" t="s">
         <v>5</v>
       </c>
       <c r="G3" s="11">
@@ -3108,33 +3108,33 @@
       <c r="I3" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="J3" s="104">
+      <c r="J3" s="92">
         <v>2</v>
       </c>
-      <c r="K3" s="123">
-        <v>1</v>
-      </c>
-      <c r="L3" s="127">
-        <v>1</v>
-      </c>
-      <c r="M3" s="127">
-        <v>1</v>
-      </c>
-      <c r="N3" s="127">
+      <c r="K3" s="95">
+        <v>1</v>
+      </c>
+      <c r="L3" s="99">
+        <v>1</v>
+      </c>
+      <c r="M3" s="99">
+        <v>1</v>
+      </c>
+      <c r="N3" s="99">
         <v>0</v>
       </c>
-      <c r="O3" s="104">
+      <c r="O3" s="92">
         <v>1</v>
       </c>
       <c r="P3" s="117">
-        <v>44778</v>
+        <v>44779</v>
       </c>
       <c r="Q3" s="114">
         <v>44783</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="96"/>
+      <c r="A4" s="90"/>
       <c r="B4" s="17">
         <v>2</v>
       </c>
@@ -3145,7 +3145,7 @@
         <v>39</v>
       </c>
       <c r="E4" s="7"/>
-      <c r="F4" s="90"/>
+      <c r="F4" s="105"/>
       <c r="G4" s="8">
         <v>39571</v>
       </c>
@@ -3155,17 +3155,17 @@
       <c r="I4" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="J4" s="105"/>
-      <c r="K4" s="124"/>
-      <c r="L4" s="128"/>
-      <c r="M4" s="128"/>
-      <c r="N4" s="128"/>
-      <c r="O4" s="105"/>
+      <c r="J4" s="93"/>
+      <c r="K4" s="96"/>
+      <c r="L4" s="100"/>
+      <c r="M4" s="100"/>
+      <c r="N4" s="100"/>
+      <c r="O4" s="93"/>
       <c r="P4" s="118"/>
       <c r="Q4" s="115"/>
     </row>
     <row r="5" spans="1:17" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="96"/>
+      <c r="A5" s="90"/>
       <c r="B5" s="17">
         <v>3</v>
       </c>
@@ -3176,7 +3176,7 @@
         <v>37</v>
       </c>
       <c r="E5" s="7"/>
-      <c r="F5" s="90"/>
+      <c r="F5" s="105"/>
       <c r="G5" s="8">
         <v>39459</v>
       </c>
@@ -3186,17 +3186,17 @@
       <c r="I5" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="J5" s="105"/>
-      <c r="K5" s="124"/>
-      <c r="L5" s="128"/>
-      <c r="M5" s="128"/>
-      <c r="N5" s="128"/>
-      <c r="O5" s="105"/>
+      <c r="J5" s="93"/>
+      <c r="K5" s="96"/>
+      <c r="L5" s="100"/>
+      <c r="M5" s="100"/>
+      <c r="N5" s="100"/>
+      <c r="O5" s="93"/>
       <c r="P5" s="118"/>
       <c r="Q5" s="115"/>
     </row>
     <row r="6" spans="1:17" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="96"/>
+      <c r="A6" s="90"/>
       <c r="B6" s="17">
         <v>4</v>
       </c>
@@ -3207,7 +3207,7 @@
         <v>39</v>
       </c>
       <c r="E6" s="7"/>
-      <c r="F6" s="90"/>
+      <c r="F6" s="105"/>
       <c r="G6" s="8">
         <v>40505</v>
       </c>
@@ -3217,17 +3217,17 @@
       <c r="I6" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="J6" s="105"/>
-      <c r="K6" s="124"/>
-      <c r="L6" s="128"/>
-      <c r="M6" s="128"/>
-      <c r="N6" s="128"/>
-      <c r="O6" s="105"/>
+      <c r="J6" s="93"/>
+      <c r="K6" s="96"/>
+      <c r="L6" s="100"/>
+      <c r="M6" s="100"/>
+      <c r="N6" s="100"/>
+      <c r="O6" s="93"/>
       <c r="P6" s="118"/>
       <c r="Q6" s="115"/>
     </row>
     <row r="7" spans="1:17" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="97"/>
+      <c r="A7" s="91"/>
       <c r="B7" s="18">
         <v>5</v>
       </c>
@@ -3238,7 +3238,7 @@
         <v>40</v>
       </c>
       <c r="E7" s="13"/>
-      <c r="F7" s="91"/>
+      <c r="F7" s="106"/>
       <c r="G7" s="14">
         <v>41149</v>
       </c>
@@ -3248,17 +3248,17 @@
       <c r="I7" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="J7" s="106"/>
-      <c r="K7" s="126"/>
-      <c r="L7" s="130"/>
-      <c r="M7" s="130"/>
-      <c r="N7" s="130"/>
-      <c r="O7" s="106"/>
+      <c r="J7" s="94"/>
+      <c r="K7" s="98"/>
+      <c r="L7" s="102"/>
+      <c r="M7" s="102"/>
+      <c r="N7" s="102"/>
+      <c r="O7" s="94"/>
       <c r="P7" s="118"/>
       <c r="Q7" s="115"/>
     </row>
     <row r="8" spans="1:17" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A8" s="95">
+      <c r="A8" s="89">
         <v>2</v>
       </c>
       <c r="B8" s="16">
@@ -3271,7 +3271,7 @@
       <c r="E8" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="F8" s="89" t="s">
+      <c r="F8" s="104" t="s">
         <v>90</v>
       </c>
       <c r="G8" s="11">
@@ -3283,29 +3283,29 @@
       <c r="I8" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="J8" s="104">
+      <c r="J8" s="92">
         <v>2</v>
       </c>
-      <c r="K8" s="123">
-        <v>1</v>
-      </c>
-      <c r="L8" s="127">
+      <c r="K8" s="95">
+        <v>1</v>
+      </c>
+      <c r="L8" s="99">
         <v>0</v>
       </c>
-      <c r="M8" s="127">
-        <v>1</v>
-      </c>
-      <c r="N8" s="127">
+      <c r="M8" s="99">
+        <v>1</v>
+      </c>
+      <c r="N8" s="99">
         <v>0</v>
       </c>
-      <c r="O8" s="104">
+      <c r="O8" s="92">
         <v>0</v>
       </c>
       <c r="P8" s="118"/>
       <c r="Q8" s="115"/>
     </row>
     <row r="9" spans="1:17" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A9" s="96"/>
+      <c r="A9" s="90"/>
       <c r="B9" s="17">
         <v>2</v>
       </c>
@@ -3316,7 +3316,7 @@
         <v>44</v>
       </c>
       <c r="E9" s="7"/>
-      <c r="F9" s="90"/>
+      <c r="F9" s="105"/>
       <c r="G9" s="8">
         <v>39826</v>
       </c>
@@ -3326,17 +3326,17 @@
       <c r="I9" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="J9" s="105"/>
-      <c r="K9" s="124"/>
-      <c r="L9" s="128"/>
-      <c r="M9" s="128"/>
-      <c r="N9" s="128"/>
-      <c r="O9" s="105"/>
+      <c r="J9" s="93"/>
+      <c r="K9" s="96"/>
+      <c r="L9" s="100"/>
+      <c r="M9" s="100"/>
+      <c r="N9" s="100"/>
+      <c r="O9" s="93"/>
       <c r="P9" s="118"/>
       <c r="Q9" s="115"/>
     </row>
     <row r="10" spans="1:17" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A10" s="96"/>
+      <c r="A10" s="90"/>
       <c r="B10" s="17">
         <v>3</v>
       </c>
@@ -3347,7 +3347,7 @@
         <v>44</v>
       </c>
       <c r="E10" s="7"/>
-      <c r="F10" s="90"/>
+      <c r="F10" s="105"/>
       <c r="G10" s="8">
         <v>40291</v>
       </c>
@@ -3357,17 +3357,17 @@
       <c r="I10" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="J10" s="105"/>
-      <c r="K10" s="124"/>
-      <c r="L10" s="128"/>
-      <c r="M10" s="128"/>
-      <c r="N10" s="128"/>
-      <c r="O10" s="105"/>
+      <c r="J10" s="93"/>
+      <c r="K10" s="96"/>
+      <c r="L10" s="100"/>
+      <c r="M10" s="100"/>
+      <c r="N10" s="100"/>
+      <c r="O10" s="93"/>
       <c r="P10" s="118"/>
       <c r="Q10" s="115"/>
     </row>
     <row r="11" spans="1:17" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A11" s="96"/>
+      <c r="A11" s="90"/>
       <c r="B11" s="17">
         <v>4</v>
       </c>
@@ -3378,7 +3378,7 @@
         <v>44</v>
       </c>
       <c r="E11" s="7"/>
-      <c r="F11" s="90"/>
+      <c r="F11" s="105"/>
       <c r="G11" s="8">
         <v>40497</v>
       </c>
@@ -3388,17 +3388,17 @@
       <c r="I11" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="J11" s="105"/>
-      <c r="K11" s="124"/>
-      <c r="L11" s="128"/>
-      <c r="M11" s="128"/>
-      <c r="N11" s="128"/>
-      <c r="O11" s="105"/>
+      <c r="J11" s="93"/>
+      <c r="K11" s="96"/>
+      <c r="L11" s="100"/>
+      <c r="M11" s="100"/>
+      <c r="N11" s="100"/>
+      <c r="O11" s="93"/>
       <c r="P11" s="118"/>
       <c r="Q11" s="115"/>
     </row>
     <row r="12" spans="1:17" ht="26.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="107"/>
+      <c r="A12" s="130"/>
       <c r="B12" s="71">
         <v>5</v>
       </c>
@@ -3409,7 +3409,7 @@
         <v>44</v>
       </c>
       <c r="E12" s="73"/>
-      <c r="F12" s="90"/>
+      <c r="F12" s="105"/>
       <c r="G12" s="74">
         <v>39894</v>
       </c>
@@ -3419,17 +3419,17 @@
       <c r="I12" s="75" t="s">
         <v>124</v>
       </c>
-      <c r="J12" s="113"/>
-      <c r="K12" s="125"/>
-      <c r="L12" s="129"/>
-      <c r="M12" s="129"/>
-      <c r="N12" s="129"/>
-      <c r="O12" s="113"/>
+      <c r="J12" s="103"/>
+      <c r="K12" s="97"/>
+      <c r="L12" s="101"/>
+      <c r="M12" s="101"/>
+      <c r="N12" s="101"/>
+      <c r="O12" s="103"/>
       <c r="P12" s="118"/>
       <c r="Q12" s="115"/>
     </row>
     <row r="13" spans="1:17" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="97"/>
+      <c r="A13" s="91"/>
       <c r="B13" s="18">
         <v>6</v>
       </c>
@@ -3440,7 +3440,7 @@
         <v>44</v>
       </c>
       <c r="E13" s="13"/>
-      <c r="F13" s="91"/>
+      <c r="F13" s="106"/>
       <c r="G13" s="14">
         <v>40231</v>
       </c>
@@ -3450,17 +3450,17 @@
       <c r="I13" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="J13" s="106"/>
-      <c r="K13" s="126"/>
-      <c r="L13" s="130"/>
-      <c r="M13" s="130"/>
-      <c r="N13" s="130"/>
-      <c r="O13" s="106"/>
+      <c r="J13" s="94"/>
+      <c r="K13" s="98"/>
+      <c r="L13" s="102"/>
+      <c r="M13" s="102"/>
+      <c r="N13" s="102"/>
+      <c r="O13" s="94"/>
       <c r="P13" s="118"/>
       <c r="Q13" s="115"/>
     </row>
     <row r="14" spans="1:17" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A14" s="95">
+      <c r="A14" s="89">
         <v>3</v>
       </c>
       <c r="B14" s="16">
@@ -3473,7 +3473,7 @@
       <c r="E14" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="89" t="s">
+      <c r="F14" s="104" t="s">
         <v>51</v>
       </c>
       <c r="G14" s="11">
@@ -3485,29 +3485,29 @@
       <c r="I14" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="J14" s="104">
-        <v>1</v>
-      </c>
-      <c r="K14" s="108">
+      <c r="J14" s="92">
+        <v>1</v>
+      </c>
+      <c r="K14" s="107">
         <v>0</v>
       </c>
-      <c r="L14" s="98">
+      <c r="L14" s="109">
         <v>0</v>
       </c>
-      <c r="M14" s="98">
-        <v>1</v>
-      </c>
-      <c r="N14" s="98">
+      <c r="M14" s="109">
+        <v>1</v>
+      </c>
+      <c r="N14" s="109">
         <v>0</v>
       </c>
-      <c r="O14" s="101">
+      <c r="O14" s="123">
         <v>1</v>
       </c>
       <c r="P14" s="118"/>
       <c r="Q14" s="115"/>
     </row>
     <row r="15" spans="1:17" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="97"/>
+      <c r="A15" s="91"/>
       <c r="B15" s="18">
         <v>2</v>
       </c>
@@ -3520,7 +3520,7 @@
       <c r="E15" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="F15" s="91"/>
+      <c r="F15" s="106"/>
       <c r="G15" s="14">
         <v>37459</v>
       </c>
@@ -3530,17 +3530,17 @@
       <c r="I15" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="J15" s="106"/>
-      <c r="K15" s="110"/>
-      <c r="L15" s="100"/>
-      <c r="M15" s="100"/>
-      <c r="N15" s="100"/>
-      <c r="O15" s="103"/>
+      <c r="J15" s="94"/>
+      <c r="K15" s="108"/>
+      <c r="L15" s="111"/>
+      <c r="M15" s="111"/>
+      <c r="N15" s="111"/>
+      <c r="O15" s="124"/>
       <c r="P15" s="118"/>
       <c r="Q15" s="115"/>
     </row>
     <row r="16" spans="1:17" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A16" s="95">
+      <c r="A16" s="89">
         <v>4</v>
       </c>
       <c r="B16" s="16">
@@ -3553,7 +3553,7 @@
       <c r="E16" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="F16" s="89" t="s">
+      <c r="F16" s="104" t="s">
         <v>49</v>
       </c>
       <c r="G16" s="11">
@@ -3565,29 +3565,29 @@
       <c r="I16" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="J16" s="104">
+      <c r="J16" s="92">
         <v>2</v>
       </c>
-      <c r="K16" s="108">
+      <c r="K16" s="107">
         <v>0</v>
       </c>
-      <c r="L16" s="98">
-        <v>1</v>
-      </c>
-      <c r="M16" s="98">
+      <c r="L16" s="109">
+        <v>1</v>
+      </c>
+      <c r="M16" s="109">
         <v>0</v>
       </c>
-      <c r="N16" s="98">
+      <c r="N16" s="109">
         <v>0</v>
       </c>
-      <c r="O16" s="101">
+      <c r="O16" s="123">
         <v>1</v>
       </c>
       <c r="P16" s="118"/>
       <c r="Q16" s="115"/>
     </row>
     <row r="17" spans="1:17" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A17" s="96"/>
+      <c r="A17" s="90"/>
       <c r="B17" s="17">
         <v>2</v>
       </c>
@@ -3600,7 +3600,7 @@
       <c r="E17" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="F17" s="90"/>
+      <c r="F17" s="105"/>
       <c r="G17" s="8">
         <v>38555</v>
       </c>
@@ -3610,17 +3610,17 @@
       <c r="I17" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="J17" s="105"/>
-      <c r="K17" s="109"/>
-      <c r="L17" s="99"/>
-      <c r="M17" s="99"/>
-      <c r="N17" s="99"/>
-      <c r="O17" s="102"/>
+      <c r="J17" s="93"/>
+      <c r="K17" s="125"/>
+      <c r="L17" s="110"/>
+      <c r="M17" s="110"/>
+      <c r="N17" s="110"/>
+      <c r="O17" s="126"/>
       <c r="P17" s="118"/>
       <c r="Q17" s="115"/>
     </row>
     <row r="18" spans="1:17" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A18" s="96"/>
+      <c r="A18" s="90"/>
       <c r="B18" s="17">
         <v>3</v>
       </c>
@@ -3633,7 +3633,7 @@
       <c r="E18" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="F18" s="90"/>
+      <c r="F18" s="105"/>
       <c r="G18" s="8">
         <v>37667</v>
       </c>
@@ -3643,17 +3643,17 @@
       <c r="I18" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="J18" s="105"/>
-      <c r="K18" s="109"/>
-      <c r="L18" s="99"/>
-      <c r="M18" s="99"/>
-      <c r="N18" s="99"/>
-      <c r="O18" s="102"/>
+      <c r="J18" s="93"/>
+      <c r="K18" s="125"/>
+      <c r="L18" s="110"/>
+      <c r="M18" s="110"/>
+      <c r="N18" s="110"/>
+      <c r="O18" s="126"/>
       <c r="P18" s="118"/>
       <c r="Q18" s="115"/>
     </row>
     <row r="19" spans="1:17" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="97"/>
+      <c r="A19" s="91"/>
       <c r="B19" s="18">
         <v>4</v>
       </c>
@@ -3666,7 +3666,7 @@
       <c r="E19" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="F19" s="91"/>
+      <c r="F19" s="106"/>
       <c r="G19" s="14">
         <v>37485</v>
       </c>
@@ -3676,17 +3676,17 @@
       <c r="I19" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="J19" s="106"/>
-      <c r="K19" s="110"/>
-      <c r="L19" s="100"/>
-      <c r="M19" s="100"/>
-      <c r="N19" s="100"/>
-      <c r="O19" s="103"/>
+      <c r="J19" s="94"/>
+      <c r="K19" s="108"/>
+      <c r="L19" s="111"/>
+      <c r="M19" s="111"/>
+      <c r="N19" s="111"/>
+      <c r="O19" s="124"/>
       <c r="P19" s="118"/>
       <c r="Q19" s="115"/>
     </row>
     <row r="20" spans="1:17" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A20" s="95">
+      <c r="A20" s="89">
         <v>5</v>
       </c>
       <c r="B20" s="16">
@@ -3699,7 +3699,7 @@
       <c r="E20" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="F20" s="89" t="s">
+      <c r="F20" s="104" t="s">
         <v>52</v>
       </c>
       <c r="G20" s="11">
@@ -3711,29 +3711,29 @@
       <c r="I20" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="J20" s="104">
+      <c r="J20" s="92">
         <v>2</v>
       </c>
-      <c r="K20" s="108">
-        <v>1</v>
-      </c>
-      <c r="L20" s="98">
+      <c r="K20" s="107">
+        <v>1</v>
+      </c>
+      <c r="L20" s="109">
         <v>0</v>
       </c>
-      <c r="M20" s="98">
-        <v>1</v>
-      </c>
-      <c r="N20" s="98">
-        <v>1</v>
-      </c>
-      <c r="O20" s="101">
+      <c r="M20" s="109">
+        <v>1</v>
+      </c>
+      <c r="N20" s="109">
+        <v>1</v>
+      </c>
+      <c r="O20" s="123">
         <v>1</v>
       </c>
       <c r="P20" s="118"/>
       <c r="Q20" s="115"/>
     </row>
     <row r="21" spans="1:17" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A21" s="96"/>
+      <c r="A21" s="90"/>
       <c r="B21" s="17">
         <v>2</v>
       </c>
@@ -3744,7 +3744,7 @@
         <v>69</v>
       </c>
       <c r="E21" s="7"/>
-      <c r="F21" s="90"/>
+      <c r="F21" s="105"/>
       <c r="G21" s="8">
         <v>40016</v>
       </c>
@@ -3754,17 +3754,17 @@
       <c r="I21" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="J21" s="105"/>
-      <c r="K21" s="109"/>
-      <c r="L21" s="99"/>
-      <c r="M21" s="99"/>
-      <c r="N21" s="99"/>
-      <c r="O21" s="102"/>
+      <c r="J21" s="93"/>
+      <c r="K21" s="125"/>
+      <c r="L21" s="110"/>
+      <c r="M21" s="110"/>
+      <c r="N21" s="110"/>
+      <c r="O21" s="126"/>
       <c r="P21" s="118"/>
       <c r="Q21" s="115"/>
     </row>
     <row r="22" spans="1:17" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="97"/>
+      <c r="A22" s="91"/>
       <c r="B22" s="18">
         <v>3</v>
       </c>
@@ -3775,7 +3775,7 @@
         <v>70</v>
       </c>
       <c r="E22" s="13"/>
-      <c r="F22" s="91"/>
+      <c r="F22" s="106"/>
       <c r="G22" s="14">
         <v>40224</v>
       </c>
@@ -3785,12 +3785,12 @@
       <c r="I22" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="J22" s="106"/>
-      <c r="K22" s="110"/>
-      <c r="L22" s="100"/>
-      <c r="M22" s="100"/>
-      <c r="N22" s="100"/>
-      <c r="O22" s="103"/>
+      <c r="J22" s="94"/>
+      <c r="K22" s="108"/>
+      <c r="L22" s="111"/>
+      <c r="M22" s="111"/>
+      <c r="N22" s="111"/>
+      <c r="O22" s="124"/>
       <c r="P22" s="118"/>
       <c r="Q22" s="115"/>
     </row>
@@ -3843,6 +3843,35 @@
     </row>
   </sheetData>
   <mergeCells count="45">
+    <mergeCell ref="F16:F19"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="N16:N19"/>
+    <mergeCell ref="O16:O19"/>
+    <mergeCell ref="J16:J19"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="K20:K22"/>
+    <mergeCell ref="L20:L22"/>
+    <mergeCell ref="M20:M22"/>
+    <mergeCell ref="N20:N22"/>
+    <mergeCell ref="O20:O22"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="J3:J7"/>
+    <mergeCell ref="J8:J13"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="F3:F7"/>
+    <mergeCell ref="F8:F13"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="Q3:Q23"/>
+    <mergeCell ref="P3:P23"/>
+    <mergeCell ref="J20:J22"/>
+    <mergeCell ref="K1:O1"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="M14:M15"/>
+    <mergeCell ref="N14:N15"/>
+    <mergeCell ref="O14:O15"/>
+    <mergeCell ref="K16:K19"/>
     <mergeCell ref="A20:A22"/>
     <mergeCell ref="O3:O7"/>
     <mergeCell ref="K8:K13"/>
@@ -3859,35 +3888,6 @@
     <mergeCell ref="N3:N7"/>
     <mergeCell ref="L16:L19"/>
     <mergeCell ref="M16:M19"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="J3:J7"/>
-    <mergeCell ref="J8:J13"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="F3:F7"/>
-    <mergeCell ref="F8:F13"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="Q3:Q23"/>
-    <mergeCell ref="P3:P23"/>
-    <mergeCell ref="J20:J22"/>
-    <mergeCell ref="K1:O1"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="M14:M15"/>
-    <mergeCell ref="N14:N15"/>
-    <mergeCell ref="O14:O15"/>
-    <mergeCell ref="K16:K19"/>
-    <mergeCell ref="K20:K22"/>
-    <mergeCell ref="L20:L22"/>
-    <mergeCell ref="M20:M22"/>
-    <mergeCell ref="N20:N22"/>
-    <mergeCell ref="O20:O22"/>
-    <mergeCell ref="F16:F19"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="N16:N19"/>
-    <mergeCell ref="O16:O19"/>
-    <mergeCell ref="J16:J19"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="A14:A15"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3896,12 +3896,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4114,15 +4111,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8E843C9-AFC0-407A-892D-C6431DD2F37F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D6B5C1E-8E64-4C3F-8B9C-ADE9CAA17D4A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="23dced98-c23c-4266-be03-749ab8bb2b21"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="45e2578b-5781-47e1-85a2-a2bca000d7fe"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4147,18 +4156,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D6B5C1E-8E64-4C3F-8B9C-ADE9CAA17D4A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8E843C9-AFC0-407A-892D-C6431DD2F37F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="23dced98-c23c-4266-be03-749ab8bb2b21"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="45e2578b-5781-47e1-85a2-a2bca000d7fe"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>